<commit_message>
TODO: new performance ratings
</commit_message>
<xml_diff>
--- a/data/monitors.xlsx
+++ b/data/monitors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandradeep/Desktop/MS/FrogAI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E834976C-DCBB-484F-9E69-394E19B1B049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EB27AE-ADED-384B-9D3C-6507A563B3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="212">
   <si>
     <t>name</t>
   </si>
@@ -653,6 +653,9 @@
   </si>
   <si>
     <t>Broken HDR + bad for text + 3 year burn in warranty + glossy</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -1016,20 +1019,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="15" max="15" width="41" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="16" max="16" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,43 +1046,46 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1092,44 +1098,47 @@
       <c r="D2">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>500</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>5700</v>
       </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
       <c r="L2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M2" t="s">
         <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
         <v>184</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1142,44 +1151,47 @@
       <c r="D3">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>800</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M3" t="s">
         <v>22</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
         <v>29</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1192,44 +1204,47 @@
       <c r="D4">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>800</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M4" t="s">
         <v>22</v>
       </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" t="s">
         <v>179</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1242,44 +1257,47 @@
       <c r="D5">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>20</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>800</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>28</v>
       </c>
-      <c r="K5" t="s">
-        <v>21</v>
-      </c>
       <c r="L5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M5" t="s">
         <v>22</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" t="s">
         <v>180</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1292,44 +1310,47 @@
       <c r="D6">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>38</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>900</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>28</v>
       </c>
-      <c r="K6" t="s">
-        <v>21</v>
-      </c>
       <c r="L6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M6" t="s">
         <v>22</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" t="s">
         <v>181</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1342,44 +1363,47 @@
       <c r="D7">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>34</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>20</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>870</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>28</v>
       </c>
-      <c r="K7" t="s">
-        <v>21</v>
-      </c>
       <c r="L7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M7" t="s">
         <v>22</v>
       </c>
       <c r="N7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" t="s">
         <v>182</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1392,27 +1416,27 @@
       <c r="D8">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
         <v>43</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>44</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>45</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>46</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>150</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>47</v>
       </c>
-      <c r="K8" t="s">
-        <v>21</v>
-      </c>
       <c r="L8" t="s">
         <v>21</v>
       </c>
@@ -1420,16 +1444,19 @@
         <v>21</v>
       </c>
       <c r="N8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" t="s">
         <v>48</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1442,27 +1469,27 @@
       <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>20</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>260</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>5700</v>
       </c>
-      <c r="K9" t="s">
-        <v>21</v>
-      </c>
       <c r="L9" t="s">
         <v>21</v>
       </c>
@@ -1470,16 +1497,19 @@
         <v>21</v>
       </c>
       <c r="N9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" t="s">
         <v>48</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1492,27 +1522,27 @@
       <c r="D10">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>45</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>20</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>350</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>5700</v>
       </c>
-      <c r="K10" t="s">
-        <v>21</v>
-      </c>
       <c r="L10" t="s">
         <v>21</v>
       </c>
@@ -1520,16 +1550,19 @@
         <v>21</v>
       </c>
       <c r="N10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" t="s">
         <v>53</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>55</v>
       </c>
@@ -1542,27 +1575,27 @@
       <c r="D11">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>45</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>20</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>380</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>5700</v>
       </c>
-      <c r="K11" t="s">
-        <v>21</v>
-      </c>
       <c r="L11" t="s">
         <v>21</v>
       </c>
@@ -1570,16 +1603,19 @@
         <v>21</v>
       </c>
       <c r="N11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O11" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" t="s">
         <v>48</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1592,44 +1628,47 @@
       <c r="D12">
         <v>5</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
         <v>58</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>37</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>45</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>59</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>380</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>5700</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>22</v>
       </c>
-      <c r="L12" t="s">
-        <v>21</v>
-      </c>
       <c r="M12" t="s">
         <v>21</v>
       </c>
       <c r="N12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" t="s">
         <v>60</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>48</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -1642,27 +1681,27 @@
       <c r="D13">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>63</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>45</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>38</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>400</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>5700</v>
       </c>
-      <c r="K13" t="s">
-        <v>21</v>
-      </c>
       <c r="L13" t="s">
         <v>21</v>
       </c>
@@ -1670,16 +1709,19 @@
         <v>21</v>
       </c>
       <c r="N13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" t="s">
         <v>48</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1692,44 +1734,47 @@
       <c r="D14">
         <v>5</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
         <v>17</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>18</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>45</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>20</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>420</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>66</v>
       </c>
-      <c r="K14" t="s">
-        <v>21</v>
-      </c>
       <c r="L14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" t="s">
-        <v>21</v>
-      </c>
       <c r="N14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" t="s">
         <v>183</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1742,27 +1787,27 @@
       <c r="D15">
         <v>5</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
         <v>17</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>69</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>45</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>20</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>430</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>5700</v>
       </c>
-      <c r="K15" t="s">
-        <v>21</v>
-      </c>
       <c r="L15" t="s">
         <v>21</v>
       </c>
@@ -1770,16 +1815,19 @@
         <v>21</v>
       </c>
       <c r="N15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O15" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" t="s">
         <v>48</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1792,44 +1840,47 @@
       <c r="D16">
         <v>5</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
         <v>58</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>37</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>45</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>59</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>750</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>5700</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>22</v>
       </c>
-      <c r="L16" t="s">
-        <v>21</v>
-      </c>
       <c r="M16" t="s">
         <v>21</v>
       </c>
       <c r="N16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" t="s">
         <v>60</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>48</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -1842,44 +1893,47 @@
       <c r="D17">
         <v>5</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
         <v>74</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>37</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>45</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>75</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>1000</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>5700</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>22</v>
       </c>
-      <c r="L17" t="s">
-        <v>21</v>
-      </c>
       <c r="M17" t="s">
         <v>21</v>
       </c>
       <c r="N17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" t="s">
         <v>60</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>48</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -1892,27 +1946,27 @@
       <c r="D18">
         <v>5</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
         <v>17</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>44</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>45</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>20</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>450</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>5700</v>
       </c>
-      <c r="K18" t="s">
-        <v>21</v>
-      </c>
       <c r="L18" t="s">
         <v>21</v>
       </c>
@@ -1920,16 +1974,19 @@
         <v>21</v>
       </c>
       <c r="N18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O18" t="s">
+        <v>23</v>
+      </c>
+      <c r="P18" t="s">
         <v>48</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -1942,27 +1999,27 @@
       <c r="D19">
         <v>5</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>80</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>45</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>20</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>600</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>5700</v>
       </c>
-      <c r="K19" t="s">
-        <v>21</v>
-      </c>
       <c r="L19" t="s">
         <v>21</v>
       </c>
@@ -1970,16 +2027,19 @@
         <v>21</v>
       </c>
       <c r="N19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O19" t="s">
+        <v>23</v>
+      </c>
+      <c r="P19" t="s">
         <v>48</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -1992,27 +2052,27 @@
       <c r="D20">
         <v>5</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
         <v>17</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>44</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>45</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>20</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>600</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>5700</v>
       </c>
-      <c r="K20" t="s">
-        <v>21</v>
-      </c>
       <c r="L20" t="s">
         <v>21</v>
       </c>
@@ -2020,16 +2080,19 @@
         <v>21</v>
       </c>
       <c r="N20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O20" t="s">
+        <v>23</v>
+      </c>
+      <c r="P20" t="s">
         <v>186</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>84</v>
       </c>
@@ -2042,44 +2105,47 @@
       <c r="D21">
         <v>5</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
         <v>17</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>44</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>45</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>20</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>750</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>5700</v>
       </c>
-      <c r="K21" t="s">
-        <v>21</v>
-      </c>
       <c r="L21" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" t="s">
         <v>22</v>
       </c>
-      <c r="M21" t="s">
-        <v>21</v>
-      </c>
       <c r="N21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O21" t="s">
+        <v>23</v>
+      </c>
+      <c r="P21" t="s">
         <v>208</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>86</v>
       </c>
@@ -2092,27 +2158,27 @@
       <c r="D22">
         <v>5</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
         <v>17</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>87</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>45</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>20</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>1050</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>5700</v>
       </c>
-      <c r="K22" t="s">
-        <v>21</v>
-      </c>
       <c r="L22" t="s">
         <v>21</v>
       </c>
@@ -2120,16 +2186,19 @@
         <v>21</v>
       </c>
       <c r="N22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O22" t="s">
+        <v>23</v>
+      </c>
+      <c r="P22" t="s">
         <v>185</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -2142,44 +2211,47 @@
       <c r="D23">
         <v>5</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
         <v>17</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>18</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>90</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>20</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>250</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>5700</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>22</v>
       </c>
-      <c r="L23" t="s">
-        <v>21</v>
-      </c>
       <c r="M23" t="s">
         <v>21</v>
       </c>
       <c r="N23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O23" t="s">
+        <v>23</v>
+      </c>
+      <c r="P23" t="s">
         <v>48</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -2192,44 +2264,47 @@
       <c r="D24">
         <v>3</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>18</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>90</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>38</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>300</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>5700</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>22</v>
       </c>
-      <c r="L24" t="s">
-        <v>21</v>
-      </c>
       <c r="M24" t="s">
         <v>21</v>
       </c>
       <c r="N24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O24" t="s">
+        <v>23</v>
+      </c>
+      <c r="P24" t="s">
         <v>48</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2242,44 +2317,47 @@
       <c r="D25">
         <v>7</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
         <v>26</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>95</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>90</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>38</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>350</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>5700</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>22</v>
       </c>
-      <c r="L25" t="s">
-        <v>21</v>
-      </c>
       <c r="M25" t="s">
         <v>21</v>
       </c>
       <c r="N25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O25" t="s">
+        <v>23</v>
+      </c>
+      <c r="P25" t="s">
         <v>48</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>97</v>
       </c>
@@ -2292,44 +2370,47 @@
       <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26" t="s">
         <v>58</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>37</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>90</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>59</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>450</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>98</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>22</v>
       </c>
-      <c r="L26" t="s">
-        <v>21</v>
-      </c>
       <c r="M26" t="s">
         <v>21</v>
       </c>
       <c r="N26" t="s">
+        <v>21</v>
+      </c>
+      <c r="O26" t="s">
         <v>60</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>187</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -2342,44 +2423,47 @@
       <c r="D27">
         <v>5</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
         <v>17</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>18</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>101</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>20</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>500</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>5700</v>
       </c>
-      <c r="K27" t="s">
-        <v>21</v>
-      </c>
       <c r="L27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M27" t="s">
         <v>22</v>
       </c>
       <c r="N27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O27" t="s">
+        <v>23</v>
+      </c>
+      <c r="P27" t="s">
         <v>48</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -2392,27 +2476,27 @@
       <c r="D28">
         <v>8</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
         <v>26</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>37</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>45</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>104</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>600</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>28</v>
       </c>
-      <c r="K28" t="s">
-        <v>21</v>
-      </c>
       <c r="L28" t="s">
         <v>21</v>
       </c>
@@ -2420,16 +2504,19 @@
         <v>21</v>
       </c>
       <c r="N28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P28" t="s">
         <v>188</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -2442,27 +2529,27 @@
       <c r="D29">
         <v>8</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29">
+        <v>8</v>
+      </c>
+      <c r="F29" t="s">
         <v>26</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>37</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>45</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>104</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>600</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>28</v>
       </c>
-      <c r="K29" t="s">
-        <v>21</v>
-      </c>
       <c r="L29" t="s">
         <v>21</v>
       </c>
@@ -2470,16 +2557,19 @@
         <v>21</v>
       </c>
       <c r="N29" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O29" t="s">
+        <v>23</v>
+      </c>
+      <c r="P29" t="s">
         <v>48</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>108</v>
       </c>
@@ -2492,27 +2582,27 @@
       <c r="D30">
         <v>7</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
         <v>26</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>37</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>45</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>38</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>650</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>28</v>
       </c>
-      <c r="K30" t="s">
-        <v>21</v>
-      </c>
       <c r="L30" t="s">
         <v>21</v>
       </c>
@@ -2520,16 +2610,19 @@
         <v>21</v>
       </c>
       <c r="N30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O30" t="s">
+        <v>23</v>
+      </c>
+      <c r="P30" t="s">
         <v>188</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -2542,27 +2635,27 @@
       <c r="D31">
         <v>7</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
         <v>26</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>27</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>90</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>38</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>650</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>28</v>
       </c>
-      <c r="K31" t="s">
-        <v>21</v>
-      </c>
       <c r="L31" t="s">
         <v>21</v>
       </c>
@@ -2570,16 +2663,19 @@
         <v>21</v>
       </c>
       <c r="N31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O31" t="s">
+        <v>23</v>
+      </c>
+      <c r="P31" t="s">
         <v>188</v>
       </c>
-      <c r="P31" t="s">
+      <c r="Q31" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -2592,44 +2688,47 @@
       <c r="D32">
         <v>8</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
         <v>26</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>95</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>113</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>20</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>700</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>28</v>
       </c>
-      <c r="K32" t="s">
-        <v>21</v>
-      </c>
       <c r="L32" t="s">
         <v>21</v>
       </c>
       <c r="M32" t="s">
+        <v>21</v>
+      </c>
+      <c r="N32" t="s">
         <v>22</v>
       </c>
-      <c r="N32" t="s">
-        <v>23</v>
-      </c>
       <c r="O32" t="s">
+        <v>23</v>
+      </c>
+      <c r="P32" t="s">
         <v>48</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -2642,44 +2741,47 @@
       <c r="D33">
         <v>7</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
         <v>26</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>116</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>34</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>38</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>3000</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>28</v>
       </c>
-      <c r="K33" t="s">
-        <v>21</v>
-      </c>
       <c r="L33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M33" t="s">
         <v>22</v>
       </c>
       <c r="N33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O33" t="s">
+        <v>23</v>
+      </c>
+      <c r="P33" t="s">
         <v>189</v>
       </c>
-      <c r="P33" t="s">
+      <c r="Q33" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -2692,44 +2794,47 @@
       <c r="D34">
         <v>10</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
         <v>118</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>95</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>119</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>38</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>5000</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>66</v>
       </c>
-      <c r="K34" t="s">
-        <v>21</v>
-      </c>
       <c r="L34" t="s">
         <v>21</v>
       </c>
       <c r="M34" t="s">
+        <v>21</v>
+      </c>
+      <c r="N34" t="s">
         <v>22</v>
       </c>
-      <c r="N34" t="s">
-        <v>23</v>
-      </c>
       <c r="O34" t="s">
+        <v>23</v>
+      </c>
+      <c r="P34" t="s">
         <v>190</v>
       </c>
-      <c r="P34" t="s">
+      <c r="Q34" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>121</v>
       </c>
@@ -2742,44 +2847,47 @@
       <c r="D35">
         <v>4</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
         <v>17</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>44</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>122</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>20</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>1000</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>28</v>
       </c>
-      <c r="K35" t="s">
-        <v>21</v>
-      </c>
       <c r="L35" t="s">
         <v>21</v>
       </c>
       <c r="M35" t="s">
+        <v>21</v>
+      </c>
+      <c r="N35" t="s">
         <v>22</v>
       </c>
-      <c r="N35" t="s">
-        <v>23</v>
-      </c>
       <c r="O35" t="s">
+        <v>23</v>
+      </c>
+      <c r="P35" t="s">
         <v>191</v>
       </c>
-      <c r="P35" t="s">
+      <c r="Q35" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>124</v>
       </c>
@@ -2792,44 +2900,47 @@
       <c r="D36">
         <v>4</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
         <v>17</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>44</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>122</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>20</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>1000</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>28</v>
       </c>
-      <c r="K36" t="s">
-        <v>21</v>
-      </c>
       <c r="L36" t="s">
         <v>21</v>
       </c>
       <c r="M36" t="s">
+        <v>21</v>
+      </c>
+      <c r="N36" t="s">
         <v>22</v>
       </c>
-      <c r="N36" t="s">
-        <v>23</v>
-      </c>
       <c r="O36" t="s">
+        <v>23</v>
+      </c>
+      <c r="P36" t="s">
         <v>191</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>126</v>
       </c>
@@ -2842,44 +2953,47 @@
       <c r="D37">
         <v>1.5</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37">
+        <v>1.5</v>
+      </c>
+      <c r="F37" t="s">
         <v>58</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>44</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>122</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>20</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>1700</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>28</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>22</v>
       </c>
-      <c r="L37" t="s">
-        <v>21</v>
-      </c>
       <c r="M37" t="s">
+        <v>21</v>
+      </c>
+      <c r="N37" t="s">
         <v>22</v>
       </c>
-      <c r="N37" t="s">
+      <c r="O37" t="s">
         <v>60</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>192</v>
       </c>
-      <c r="P37" t="s">
+      <c r="Q37" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>128</v>
       </c>
@@ -2892,44 +3006,47 @@
       <c r="D38">
         <v>4</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
         <v>58</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>129</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>130</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>59</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>1100</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>28</v>
-      </c>
-      <c r="K38" t="s">
-        <v>22</v>
       </c>
       <c r="L38" t="s">
         <v>22</v>
       </c>
       <c r="M38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N38" t="s">
+        <v>21</v>
+      </c>
+      <c r="O38" t="s">
         <v>60</v>
       </c>
-      <c r="O38" t="s">
+      <c r="P38" t="s">
         <v>210</v>
       </c>
-      <c r="P38" t="s">
+      <c r="Q38" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -2942,26 +3059,26 @@
       <c r="D39">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
         <v>58</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>129</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>130</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>59</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>1140</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>28</v>
-      </c>
-      <c r="K39" t="s">
-        <v>22</v>
       </c>
       <c r="L39" t="s">
         <v>22</v>
@@ -2970,16 +3087,19 @@
         <v>22</v>
       </c>
       <c r="N39" t="s">
+        <v>22</v>
+      </c>
+      <c r="O39" t="s">
         <v>60</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>194</v>
       </c>
-      <c r="P39" t="s">
+      <c r="Q39" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>134</v>
       </c>
@@ -2992,44 +3112,47 @@
       <c r="D40">
         <v>7</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
         <v>26</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>95</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>135</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>38</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>2800</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>66</v>
       </c>
-      <c r="K40" t="s">
-        <v>21</v>
-      </c>
       <c r="L40" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" t="s">
         <v>22</v>
       </c>
-      <c r="M40" t="s">
-        <v>21</v>
-      </c>
       <c r="N40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P40" t="s">
         <v>195</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>137</v>
       </c>
@@ -3042,44 +3165,47 @@
       <c r="D41">
         <v>7</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
         <v>26</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>95</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>135</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>38</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>2800</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>66</v>
       </c>
-      <c r="K41" t="s">
-        <v>21</v>
-      </c>
       <c r="L41" t="s">
+        <v>21</v>
+      </c>
+      <c r="M41" t="s">
         <v>22</v>
       </c>
-      <c r="M41" t="s">
-        <v>21</v>
-      </c>
       <c r="N41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O41" t="s">
+        <v>23</v>
+      </c>
+      <c r="P41" t="s">
         <v>195</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>138</v>
       </c>
@@ -3092,44 +3218,47 @@
       <c r="D42">
         <v>8</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42" t="s">
         <v>26</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>95</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>45</v>
       </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>20</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>500</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>66</v>
       </c>
-      <c r="K42" t="s">
-        <v>21</v>
-      </c>
       <c r="L42" t="s">
+        <v>21</v>
+      </c>
+      <c r="M42" t="s">
         <v>22</v>
       </c>
-      <c r="M42" t="s">
-        <v>21</v>
-      </c>
       <c r="N42" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O42" t="s">
+        <v>23</v>
+      </c>
+      <c r="P42" t="s">
         <v>193</v>
       </c>
-      <c r="P42" t="s">
+      <c r="Q42" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>140</v>
       </c>
@@ -3142,44 +3271,47 @@
       <c r="D43">
         <v>7</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
         <v>26</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>95</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>45</v>
       </c>
-      <c r="H43" t="s">
+      <c r="I43" t="s">
         <v>38</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>1000</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>66</v>
       </c>
-      <c r="K43" t="s">
-        <v>21</v>
-      </c>
       <c r="L43" t="s">
+        <v>21</v>
+      </c>
+      <c r="M43" t="s">
         <v>22</v>
       </c>
-      <c r="M43" t="s">
-        <v>21</v>
-      </c>
       <c r="N43" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O43" t="s">
+        <v>23</v>
+      </c>
+      <c r="P43" t="s">
         <v>196</v>
       </c>
-      <c r="P43" t="s">
+      <c r="Q43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>141</v>
       </c>
@@ -3192,27 +3324,27 @@
       <c r="D44">
         <v>3</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
         <v>43</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>44</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>45</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>142</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>280</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>47</v>
       </c>
-      <c r="K44" t="s">
-        <v>21</v>
-      </c>
       <c r="L44" t="s">
         <v>21</v>
       </c>
@@ -3220,16 +3352,19 @@
         <v>21</v>
       </c>
       <c r="N44" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O44" t="s">
+        <v>23</v>
+      </c>
+      <c r="P44" t="s">
         <v>197</v>
       </c>
-      <c r="P44" t="s">
+      <c r="Q44" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>144</v>
       </c>
@@ -3242,27 +3377,27 @@
       <c r="D45">
         <v>3</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
         <v>43</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>145</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>45</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>46</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>300</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>47</v>
       </c>
-      <c r="K45" t="s">
-        <v>21</v>
-      </c>
       <c r="L45" t="s">
         <v>21</v>
       </c>
@@ -3270,16 +3405,19 @@
         <v>21</v>
       </c>
       <c r="N45" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O45" t="s">
+        <v>23</v>
+      </c>
+      <c r="P45" t="s">
         <v>198</v>
       </c>
-      <c r="P45" t="s">
+      <c r="Q45" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>147</v>
       </c>
@@ -3292,27 +3430,27 @@
       <c r="D46">
         <v>3</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
         <v>43</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>87</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>148</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>46</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>600</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>47</v>
       </c>
-      <c r="K46" t="s">
-        <v>21</v>
-      </c>
       <c r="L46" t="s">
         <v>21</v>
       </c>
@@ -3320,16 +3458,19 @@
         <v>21</v>
       </c>
       <c r="N46" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O46" t="s">
+        <v>23</v>
+      </c>
+      <c r="P46" t="s">
         <v>199</v>
       </c>
-      <c r="P46" t="s">
+      <c r="Q46" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>150</v>
       </c>
@@ -3342,27 +3483,27 @@
       <c r="D47">
         <v>3</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" t="s">
         <v>43</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>151</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>45</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>46</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>830</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>47</v>
       </c>
-      <c r="K47" t="s">
-        <v>21</v>
-      </c>
       <c r="L47" t="s">
         <v>21</v>
       </c>
@@ -3370,16 +3511,19 @@
         <v>21</v>
       </c>
       <c r="N47" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O47" t="s">
+        <v>23</v>
+      </c>
+      <c r="P47" t="s">
         <v>48</v>
       </c>
-      <c r="P47" t="s">
+      <c r="Q47" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>153</v>
       </c>
@@ -3392,27 +3536,27 @@
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
         <v>17</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>154</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>45</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>20</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>250</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>66</v>
       </c>
-      <c r="K48" t="s">
-        <v>21</v>
-      </c>
       <c r="L48" t="s">
         <v>21</v>
       </c>
@@ -3420,16 +3564,19 @@
         <v>21</v>
       </c>
       <c r="N48" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O48" t="s">
+        <v>23</v>
+      </c>
+      <c r="P48" t="s">
         <v>155</v>
       </c>
-      <c r="P48" t="s">
+      <c r="Q48" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>157</v>
       </c>
@@ -3442,27 +3589,27 @@
       <c r="D49">
         <v>8</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
         <v>26</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>95</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>45</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>20</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>300</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>66</v>
       </c>
-      <c r="K49" t="s">
-        <v>21</v>
-      </c>
       <c r="L49" t="s">
         <v>21</v>
       </c>
@@ -3470,16 +3617,19 @@
         <v>21</v>
       </c>
       <c r="N49" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O49" t="s">
+        <v>23</v>
+      </c>
+      <c r="P49" t="s">
         <v>155</v>
       </c>
-      <c r="P49" t="s">
+      <c r="Q49" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>159</v>
       </c>
@@ -3492,27 +3642,27 @@
       <c r="D50">
         <v>8</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
         <v>26</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>95</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>45</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>20</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>400</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>66</v>
       </c>
-      <c r="K50" t="s">
-        <v>21</v>
-      </c>
       <c r="L50" t="s">
         <v>21</v>
       </c>
@@ -3520,16 +3670,19 @@
         <v>21</v>
       </c>
       <c r="N50" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O50" t="s">
+        <v>23</v>
+      </c>
+      <c r="P50" t="s">
         <v>200</v>
       </c>
-      <c r="P50" t="s">
+      <c r="Q50" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>160</v>
       </c>
@@ -3542,44 +3695,47 @@
       <c r="D51">
         <v>5</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51" t="s">
         <v>58</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>95</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>45</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>59</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>450</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>66</v>
       </c>
-      <c r="K51" t="s">
+      <c r="L51" t="s">
         <v>22</v>
       </c>
-      <c r="L51" t="s">
-        <v>21</v>
-      </c>
       <c r="M51" t="s">
         <v>21</v>
       </c>
       <c r="N51" t="s">
+        <v>21</v>
+      </c>
+      <c r="O51" t="s">
         <v>60</v>
       </c>
-      <c r="O51" t="s">
+      <c r="P51" t="s">
         <v>200</v>
       </c>
-      <c r="P51" t="s">
+      <c r="Q51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>161</v>
       </c>
@@ -3592,27 +3748,27 @@
       <c r="D52">
         <v>8</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
         <v>26</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>95</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>45</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>20</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>450</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>66</v>
       </c>
-      <c r="K52" t="s">
-        <v>21</v>
-      </c>
       <c r="L52" t="s">
         <v>21</v>
       </c>
@@ -3620,16 +3776,19 @@
         <v>21</v>
       </c>
       <c r="N52" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O52" t="s">
+        <v>23</v>
+      </c>
+      <c r="P52" t="s">
         <v>209</v>
       </c>
-      <c r="P52" t="s">
+      <c r="Q52" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>163</v>
       </c>
@@ -3642,44 +3801,47 @@
       <c r="D53">
         <v>5</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53" t="s">
         <v>58</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>95</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>45</v>
       </c>
-      <c r="H53" t="s">
+      <c r="I53" t="s">
         <v>59</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>480</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>66</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>22</v>
       </c>
-      <c r="L53" t="s">
-        <v>21</v>
-      </c>
       <c r="M53" t="s">
         <v>21</v>
       </c>
       <c r="N53" t="s">
+        <v>21</v>
+      </c>
+      <c r="O53" t="s">
         <v>60</v>
       </c>
-      <c r="O53" t="s">
+      <c r="P53" t="s">
         <v>201</v>
       </c>
-      <c r="P53" t="s">
+      <c r="Q53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>164</v>
       </c>
@@ -3692,27 +3854,27 @@
       <c r="D54">
         <v>7</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54">
+        <v>7</v>
+      </c>
+      <c r="F54" t="s">
         <v>26</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>95</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>45</v>
       </c>
-      <c r="H54" t="s">
+      <c r="I54" t="s">
         <v>38</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>450</v>
       </c>
-      <c r="J54" t="s">
+      <c r="K54" t="s">
         <v>66</v>
       </c>
-      <c r="K54" t="s">
-        <v>21</v>
-      </c>
       <c r="L54" t="s">
         <v>21</v>
       </c>
@@ -3720,16 +3882,19 @@
         <v>21</v>
       </c>
       <c r="N54" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O54" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="P54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>165</v>
       </c>
@@ -3742,27 +3907,27 @@
       <c r="D55">
         <v>7</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55">
+        <v>7</v>
+      </c>
+      <c r="F55" t="s">
         <v>166</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>95</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>45</v>
       </c>
-      <c r="H55" t="s">
+      <c r="I55" t="s">
         <v>104</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>600</v>
       </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>66</v>
       </c>
-      <c r="K55" t="s">
-        <v>21</v>
-      </c>
       <c r="L55" t="s">
         <v>21</v>
       </c>
@@ -3770,16 +3935,19 @@
         <v>21</v>
       </c>
       <c r="N55" t="s">
+        <v>21</v>
+      </c>
+      <c r="O55" t="s">
         <v>167</v>
       </c>
-      <c r="O55" t="s">
+      <c r="P55" t="s">
         <v>202</v>
       </c>
-      <c r="P55" t="s">
+      <c r="Q55" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>168</v>
       </c>
@@ -3792,27 +3960,27 @@
       <c r="D56">
         <v>8</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56">
+        <v>8</v>
+      </c>
+      <c r="F56" t="s">
         <v>26</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>95</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>169</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>20</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>600</v>
       </c>
-      <c r="J56" t="s">
+      <c r="K56" t="s">
         <v>66</v>
       </c>
-      <c r="K56" t="s">
-        <v>21</v>
-      </c>
       <c r="L56" t="s">
         <v>21</v>
       </c>
@@ -3820,16 +3988,19 @@
         <v>21</v>
       </c>
       <c r="N56" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O56" t="s">
+        <v>23</v>
+      </c>
+      <c r="P56" t="s">
         <v>205</v>
       </c>
-      <c r="P56" t="s">
+      <c r="Q56" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>171</v>
       </c>
@@ -3842,27 +4013,27 @@
       <c r="D57">
         <v>7</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57">
+        <v>7</v>
+      </c>
+      <c r="F57" t="s">
         <v>26</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>95</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>45</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>38</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>700</v>
       </c>
-      <c r="J57" t="s">
+      <c r="K57" t="s">
         <v>66</v>
       </c>
-      <c r="K57" t="s">
-        <v>21</v>
-      </c>
       <c r="L57" t="s">
         <v>21</v>
       </c>
@@ -3870,16 +4041,19 @@
         <v>21</v>
       </c>
       <c r="N57" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O57" t="s">
+        <v>23</v>
+      </c>
+      <c r="P57" t="s">
         <v>203</v>
       </c>
-      <c r="P57" t="s">
+      <c r="Q57" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>172</v>
       </c>
@@ -3892,27 +4066,27 @@
       <c r="D58">
         <v>7</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58">
+        <v>7</v>
+      </c>
+      <c r="F58" t="s">
         <v>26</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>95</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>169</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>38</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>850</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>66</v>
       </c>
-      <c r="K58" t="s">
-        <v>21</v>
-      </c>
       <c r="L58" t="s">
         <v>21</v>
       </c>
@@ -3920,16 +4094,19 @@
         <v>21</v>
       </c>
       <c r="N58" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O58" t="s">
+        <v>23</v>
+      </c>
+      <c r="P58" t="s">
         <v>204</v>
       </c>
-      <c r="P58" t="s">
+      <c r="Q58" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>174</v>
       </c>
@@ -3942,27 +4119,27 @@
       <c r="D59">
         <v>10</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
         <v>175</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>95</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>45</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>20</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>1300</v>
       </c>
-      <c r="J59" t="s">
+      <c r="K59" t="s">
         <v>66</v>
       </c>
-      <c r="K59" t="s">
-        <v>21</v>
-      </c>
       <c r="L59" t="s">
         <v>21</v>
       </c>
@@ -3970,16 +4147,19 @@
         <v>21</v>
       </c>
       <c r="N59" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O59" t="s">
+        <v>23</v>
+      </c>
+      <c r="P59" t="s">
         <v>206</v>
       </c>
-      <c r="P59" t="s">
+      <c r="Q59" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>176</v>
       </c>
@@ -3992,44 +4172,47 @@
       <c r="D60">
         <v>5</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60">
+        <v>5</v>
+      </c>
+      <c r="F60" t="s">
         <v>74</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>37</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>45</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>75</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>1400</v>
       </c>
-      <c r="J60" t="s">
+      <c r="K60" t="s">
         <v>66</v>
       </c>
-      <c r="K60" t="s">
+      <c r="L60" t="s">
         <v>22</v>
       </c>
-      <c r="L60" t="s">
-        <v>21</v>
-      </c>
       <c r="M60" t="s">
         <v>21</v>
       </c>
       <c r="N60" t="s">
+        <v>21</v>
+      </c>
+      <c r="O60" t="s">
         <v>60</v>
       </c>
-      <c r="O60" t="s">
+      <c r="P60" t="s">
         <v>201</v>
       </c>
-      <c r="P60" t="s">
+      <c r="Q60" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>177</v>
       </c>
@@ -4042,27 +4225,27 @@
       <c r="D61">
         <v>10</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
         <v>175</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>95</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>45</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>20</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>1600</v>
       </c>
-      <c r="J61" t="s">
+      <c r="K61" t="s">
         <v>66</v>
       </c>
-      <c r="K61" t="s">
-        <v>21</v>
-      </c>
       <c r="L61" t="s">
         <v>21</v>
       </c>
@@ -4070,12 +4253,15 @@
         <v>21</v>
       </c>
       <c r="N61" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="O61" t="s">
+        <v>23</v>
+      </c>
+      <c r="P61" t="s">
         <v>207</v>
       </c>
-      <c r="P61" t="s">
+      <c r="Q61" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TODO: min and sd
</commit_message>
<xml_diff>
--- a/data/monitors.xlsx
+++ b/data/monitors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandradeep/Desktop/MS/FrogAI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE4AF68-7428-2A4F-9131-D6E2CDFE3D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D3A552-8184-024C-A050-D8F30E76278C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1369,10 +1369,10 @@
         <v>7</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I6" t="s">
         <v>31</v>
@@ -1803,7 +1803,7 @@
         <v>2</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H13">
         <v>3</v>
@@ -2485,7 +2485,7 @@
         <v>2</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H24">
         <v>3</v>
@@ -2547,10 +2547,10 @@
         <v>2</v>
       </c>
       <c r="G25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I25" t="s">
         <v>31</v>
@@ -2857,10 +2857,10 @@
         <v>2</v>
       </c>
       <c r="G30">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H30">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I30" t="s">
         <v>31</v>
@@ -2919,10 +2919,10 @@
         <v>2</v>
       </c>
       <c r="G31">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H31">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I31" t="s">
         <v>31</v>
@@ -3043,10 +3043,10 @@
         <v>8</v>
       </c>
       <c r="G33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I33" t="s">
         <v>31</v>
@@ -3291,7 +3291,7 @@
         <v>3</v>
       </c>
       <c r="G37">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H37">
         <v>1.5</v>
@@ -3477,10 +3477,10 @@
         <v>3.5</v>
       </c>
       <c r="G40">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H40">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I40" t="s">
         <v>31</v>
@@ -3539,10 +3539,10 @@
         <v>3.5</v>
       </c>
       <c r="G41">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H41">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I41" t="s">
         <v>31</v>
@@ -3663,10 +3663,10 @@
         <v>2</v>
       </c>
       <c r="G43">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H43">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I43" t="s">
         <v>31</v>
@@ -4345,10 +4345,10 @@
         <v>2</v>
       </c>
       <c r="G54">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H54">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I54" t="s">
         <v>31</v>
@@ -4407,10 +4407,10 @@
         <v>2</v>
       </c>
       <c r="G55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I55" t="s">
         <v>196</v>
@@ -4531,10 +4531,10 @@
         <v>2</v>
       </c>
       <c r="G57">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H57">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I57" t="s">
         <v>31</v>
@@ -4593,10 +4593,10 @@
         <v>2</v>
       </c>
       <c r="G58">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H58">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I58" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
tuned algorithm + added esports
</commit_message>
<xml_diff>
--- a/data/monitors.xlsx
+++ b/data/monitors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandradeep/Desktop/MS/FrogAI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D3A552-8184-024C-A050-D8F30E76278C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A826DC7-DB9E-174B-9D5B-9A40F3A71A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="212">
   <si>
     <t>name</t>
   </si>
@@ -82,9 +82,6 @@
     <t>reviews</t>
   </si>
   <si>
-    <t>CoolerMaster GP27Q</t>
-  </si>
-  <si>
     <t>2560x1440</t>
   </si>
   <si>
@@ -106,12 +103,6 @@
     <t>Wide</t>
   </si>
   <si>
-    <t>VRR+HDR flickering + other firmware issues</t>
-  </si>
-  <si>
-    <t>TFTCentral,https://tftcentral.co.uk/reviews/cooler-master-tempest-gp27q;Hardware Unboxed,https://www.youtube.com/watch?v=G6MS45GqcJ4</t>
-  </si>
-  <si>
     <t>CoolerMaster GP27U</t>
   </si>
   <si>
@@ -487,9 +478,6 @@
     <t>RTINGS,https://www.rtings.com/monitor/reviews/dell/alienware-aw3423dw;Hardware Unboxed,https://www.youtube.com/watch?v=YleSuwK8vR4</t>
   </si>
   <si>
-    <t>LG 32ep950</t>
-  </si>
-  <si>
     <t>Inkjet OLED</t>
   </si>
   <si>
@@ -665,6 +653,9 @@
   </si>
   <si>
     <t>RTINGS,https://www.rtings.com/monitor/reviews/apple/studio-display</t>
+  </si>
+  <si>
+    <t>LG 32EP950</t>
   </si>
 </sst>
 </file>
@@ -1028,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T61"/>
+  <dimension ref="A1:T60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1103,10 +1094,10 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>6.3</v>
+        <v>6.25</v>
       </c>
       <c r="C2">
         <v>6.5</v>
@@ -1121,51 +1112,51 @@
         <v>7</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
       <c r="M2">
-        <v>500</v>
-      </c>
-      <c r="N2">
-        <v>5700</v>
+        <v>800</v>
+      </c>
+      <c r="N2" t="s">
+        <v>30</v>
       </c>
       <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" t="s">
-        <v>27</v>
-      </c>
       <c r="S2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="T2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>6.25</v>
@@ -1189,34 +1180,34 @@
         <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
         <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
       </c>
       <c r="M3">
         <v>800</v>
       </c>
       <c r="N3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R3" t="s">
         <v>26</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" t="s">
-        <v>27</v>
       </c>
       <c r="S3" t="s">
         <v>34</v>
@@ -1251,54 +1242,54 @@
         <v>8</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" t="s">
         <v>23</v>
-      </c>
-      <c r="L4" t="s">
-        <v>24</v>
       </c>
       <c r="M4">
         <v>800</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="s">
         <v>25</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" t="s">
-        <v>27</v>
-      </c>
       <c r="S4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B5">
-        <v>6.25</v>
+        <v>5.8</v>
       </c>
       <c r="C5">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -1313,54 +1304,54 @@
         <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="M5">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="N5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="s">
         <v>25</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+      <c r="R5" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" t="s">
-        <v>27</v>
-      </c>
       <c r="S5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6">
-        <v>5.8</v>
+        <v>6.25</v>
       </c>
       <c r="C6">
-        <v>4.5</v>
+        <v>6.5</v>
       </c>
       <c r="D6">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>7</v>
@@ -1375,34 +1366,34 @@
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="K6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="M6">
-        <v>900</v>
+        <v>870</v>
       </c>
       <c r="N6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
         <v>25</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" t="s">
         <v>26</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>26</v>
-      </c>
-      <c r="R6" t="s">
-        <v>27</v>
       </c>
       <c r="S6" t="s">
         <v>46</v>
@@ -1416,134 +1407,134 @@
         <v>48</v>
       </c>
       <c r="B7">
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="C7">
         <v>6.5</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>1.75</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="M7">
-        <v>870</v>
+        <v>150</v>
       </c>
       <c r="N7" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="O7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R7" t="s">
         <v>26</v>
       </c>
-      <c r="Q7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R7" t="s">
-        <v>27</v>
-      </c>
       <c r="S7" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="T7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <v>6.3</v>
+      </c>
+      <c r="C8">
+        <v>5.5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
         <v>51</v>
       </c>
-      <c r="B8">
-        <v>7.5</v>
-      </c>
-      <c r="C8">
-        <v>6.5</v>
-      </c>
-      <c r="D8">
-        <v>1.75</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="I8" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8">
+        <v>260</v>
+      </c>
+      <c r="N8">
+        <v>5700</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S8" t="s">
         <v>54</v>
       </c>
-      <c r="L8" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8">
-        <v>150</v>
-      </c>
-      <c r="N8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>25</v>
-      </c>
-      <c r="R8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>57</v>
-      </c>
-      <c r="T8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9">
         <v>6.3</v>
       </c>
       <c r="C9">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1561,37 +1552,37 @@
         <v>5</v>
       </c>
       <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" t="s">
         <v>21</v>
       </c>
-      <c r="J9" t="s">
-        <v>22</v>
-      </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M9">
-        <v>260</v>
+        <v>350</v>
       </c>
       <c r="N9">
         <v>5700</v>
       </c>
       <c r="O9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T9" t="s">
         <v>60</v>
@@ -1605,16 +1596,16 @@
         <v>6.3</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10">
         <v>5</v>
@@ -1623,78 +1614,78 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" t="s">
         <v>21</v>
       </c>
-      <c r="J10" t="s">
-        <v>22</v>
-      </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M10">
-        <v>350</v>
+        <v>380</v>
       </c>
       <c r="N10">
         <v>5700</v>
       </c>
       <c r="O10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S10" t="s">
+        <v>54</v>
+      </c>
+      <c r="T10" t="s">
         <v>62</v>
-      </c>
-      <c r="T10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11">
+        <v>5.8</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
         <v>64</v>
       </c>
-      <c r="B11">
-        <v>6.3</v>
-      </c>
-      <c r="C11">
-        <v>6.5</v>
-      </c>
-      <c r="D11">
-        <v>1.75</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="I11" t="s">
-        <v>21</v>
-      </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="M11">
         <v>380</v>
@@ -1706,30 +1697,30 @@
         <v>25</v>
       </c>
       <c r="P11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R11" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="S11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B12">
-        <v>5.8</v>
+        <v>6.4</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>6.2</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1744,40 +1735,40 @@
         <v>5</v>
       </c>
       <c r="H12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="J12" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="K12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L12" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="M12">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="N12">
         <v>5700</v>
       </c>
       <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>24</v>
+      </c>
+      <c r="R12" t="s">
         <v>26</v>
       </c>
-      <c r="P12" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>25</v>
-      </c>
-      <c r="R12" t="s">
-        <v>69</v>
-      </c>
       <c r="S12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T12" t="s">
         <v>70</v>
@@ -1788,10 +1779,10 @@
         <v>71</v>
       </c>
       <c r="B13">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="C13">
-        <v>6.2</v>
+        <v>6</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1806,57 +1797,57 @@
         <v>5</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" t="s">
         <v>21</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13">
+        <v>420</v>
+      </c>
+      <c r="N13" t="s">
         <v>72</v>
       </c>
-      <c r="K13" t="s">
-        <v>54</v>
-      </c>
-      <c r="L13" t="s">
-        <v>45</v>
-      </c>
-      <c r="M13">
-        <v>400</v>
-      </c>
-      <c r="N13">
-        <v>5700</v>
-      </c>
       <c r="O13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P13" t="s">
         <v>25</v>
       </c>
       <c r="Q13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S13" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="T13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B14">
-        <v>6.3</v>
+        <v>6.6</v>
       </c>
       <c r="C14">
         <v>6</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1871,37 +1862,37 @@
         <v>5</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J14" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="K14" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14">
+        <v>430</v>
+      </c>
+      <c r="N14">
+        <v>5700</v>
+      </c>
+      <c r="O14" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>24</v>
+      </c>
+      <c r="R14" t="s">
+        <v>26</v>
+      </c>
+      <c r="S14" t="s">
         <v>54</v>
-      </c>
-      <c r="L14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14">
-        <v>420</v>
-      </c>
-      <c r="N14" t="s">
-        <v>75</v>
-      </c>
-      <c r="O14" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>25</v>
-      </c>
-      <c r="R14" t="s">
-        <v>27</v>
-      </c>
-      <c r="S14" t="s">
-        <v>76</v>
       </c>
       <c r="T14" t="s">
         <v>77</v>
@@ -1912,10 +1903,10 @@
         <v>78</v>
       </c>
       <c r="B15">
-        <v>6.6</v>
+        <v>5.8</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="D15">
         <v>1.75</v>
@@ -1933,19 +1924,19 @@
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="K15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L15" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="M15">
-        <v>430</v>
+        <v>750</v>
       </c>
       <c r="N15">
         <v>5700</v>
@@ -1954,33 +1945,33 @@
         <v>25</v>
       </c>
       <c r="P15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R15" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="S15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16">
         <v>5.8</v>
       </c>
       <c r="C16">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1995,51 +1986,51 @@
         <v>5</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K16" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L16" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="M16">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="N16">
         <v>5700</v>
       </c>
       <c r="O16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="S16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B17">
-        <v>5.8</v>
+        <v>7.5</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>6.75</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -2057,99 +2048,99 @@
         <v>5</v>
       </c>
       <c r="I17" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="J17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="K17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L17" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="M17">
-        <v>1000</v>
+        <v>450</v>
       </c>
       <c r="N17">
         <v>5700</v>
       </c>
       <c r="O17" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>24</v>
+      </c>
+      <c r="R17" t="s">
         <v>26</v>
       </c>
-      <c r="P17" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>25</v>
-      </c>
-      <c r="R17" t="s">
-        <v>69</v>
-      </c>
       <c r="S17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18">
+        <v>7.9</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" t="s">
         <v>87</v>
       </c>
-      <c r="B18">
-        <v>7.5</v>
-      </c>
-      <c r="C18">
-        <v>6.75</v>
-      </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
-      <c r="H18">
-        <v>5</v>
-      </c>
-      <c r="I18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" t="s">
-        <v>53</v>
-      </c>
       <c r="K18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M18">
-        <v>450</v>
+        <v>600</v>
       </c>
       <c r="N18">
         <v>5700</v>
       </c>
       <c r="O18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T18" t="s">
         <v>88</v>
@@ -2160,7 +2151,7 @@
         <v>89</v>
       </c>
       <c r="B19">
-        <v>7.9</v>
+        <v>7.5</v>
       </c>
       <c r="C19">
         <v>7</v>
@@ -2181,16 +2172,16 @@
         <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J19" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="K19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M19">
         <v>600</v>
@@ -2199,19 +2190,19 @@
         <v>5700</v>
       </c>
       <c r="O19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S19" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="T19" t="s">
         <v>91</v>
@@ -2225,16 +2216,16 @@
         <v>7.5</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>7.1</v>
       </c>
       <c r="D20">
         <v>2</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>5</v>
@@ -2243,34 +2234,34 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M20">
-        <v>600</v>
+        <v>750</v>
       </c>
       <c r="N20">
         <v>5700</v>
       </c>
       <c r="O20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P20" t="s">
         <v>25</v>
       </c>
       <c r="Q20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S20" t="s">
         <v>93</v>
@@ -2284,19 +2275,19 @@
         <v>95</v>
       </c>
       <c r="B21">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C21">
         <v>7.5</v>
       </c>
-      <c r="C21">
-        <v>7.1</v>
-      </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G21">
         <v>5</v>
@@ -2305,60 +2296,60 @@
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J21" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="K21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M21">
-        <v>750</v>
+        <v>1050</v>
       </c>
       <c r="N21">
         <v>5700</v>
       </c>
       <c r="O21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>24</v>
+      </c>
+      <c r="R21" t="s">
         <v>26</v>
       </c>
-      <c r="Q21" t="s">
-        <v>25</v>
-      </c>
-      <c r="R21" t="s">
-        <v>27</v>
-      </c>
       <c r="S21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="T21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B22">
-        <v>8.3000000000000007</v>
+        <v>6.3</v>
       </c>
       <c r="C22">
-        <v>7.5</v>
+        <v>1.5</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G22">
         <v>5</v>
@@ -2367,19 +2358,19 @@
         <v>5</v>
       </c>
       <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" t="s">
         <v>21</v>
       </c>
-      <c r="J22" t="s">
-        <v>99</v>
-      </c>
       <c r="K22" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="L22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M22">
-        <v>1050</v>
+        <v>250</v>
       </c>
       <c r="N22">
         <v>5700</v>
@@ -2388,16 +2379,16 @@
         <v>25</v>
       </c>
       <c r="P22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S22" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="T22" t="s">
         <v>101</v>
@@ -2411,7 +2402,7 @@
         <v>6.3</v>
       </c>
       <c r="C23">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -2426,54 +2417,54 @@
         <v>5</v>
       </c>
       <c r="H23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" t="s">
         <v>21</v>
       </c>
-      <c r="J23" t="s">
-        <v>22</v>
-      </c>
       <c r="K23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L23" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="M23">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="N23">
         <v>5700</v>
       </c>
       <c r="O23" t="s">
+        <v>25</v>
+      </c>
+      <c r="P23" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>24</v>
+      </c>
+      <c r="R23" t="s">
         <v>26</v>
       </c>
-      <c r="P23" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>25</v>
-      </c>
-      <c r="R23" t="s">
-        <v>27</v>
-      </c>
       <c r="S23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B24">
-        <v>6.3</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -2485,43 +2476,43 @@
         <v>2</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H24">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I24" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J24" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="K24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M24">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="N24">
         <v>5700</v>
       </c>
       <c r="O24" t="s">
+        <v>25</v>
+      </c>
+      <c r="P24" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>24</v>
+      </c>
+      <c r="R24" t="s">
         <v>26</v>
       </c>
-      <c r="P24" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>25</v>
-      </c>
-      <c r="R24" t="s">
-        <v>27</v>
-      </c>
       <c r="S24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T24" t="s">
         <v>106</v>
@@ -2532,81 +2523,81 @@
         <v>107</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>5.8</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="D25">
+        <v>3.5</v>
+      </c>
+      <c r="E25">
         <v>3</v>
       </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
       <c r="F25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I25" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="J25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25" t="s">
+        <v>100</v>
+      </c>
+      <c r="L25" t="s">
+        <v>65</v>
+      </c>
+      <c r="M25">
+        <v>450</v>
+      </c>
+      <c r="N25" t="s">
         <v>108</v>
       </c>
-      <c r="K25" t="s">
-        <v>103</v>
-      </c>
-      <c r="L25" t="s">
-        <v>45</v>
-      </c>
-      <c r="M25">
-        <v>350</v>
-      </c>
-      <c r="N25">
-        <v>5700</v>
-      </c>
       <c r="O25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R25" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="S25" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="T25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B26">
-        <v>5.8</v>
+        <v>6.3</v>
       </c>
       <c r="C26">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F26">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G26">
         <v>5</v>
@@ -2615,25 +2606,25 @@
         <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="J26" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="K26" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="L26" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="M26">
-        <v>450</v>
-      </c>
-      <c r="N26" t="s">
-        <v>111</v>
+        <v>500</v>
+      </c>
+      <c r="N26">
+        <v>5700</v>
       </c>
       <c r="O26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P26" t="s">
         <v>25</v>
@@ -2642,10 +2633,10 @@
         <v>25</v>
       </c>
       <c r="R26" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="S26" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="T26" t="s">
         <v>113</v>
@@ -2656,66 +2647,66 @@
         <v>114</v>
       </c>
       <c r="B27">
-        <v>6.3</v>
+        <v>5.8</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D27">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G27">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I27" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J27" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="K27" t="s">
+        <v>51</v>
+      </c>
+      <c r="L27" t="s">
         <v>115</v>
       </c>
-      <c r="L27" t="s">
-        <v>24</v>
-      </c>
       <c r="M27">
-        <v>500</v>
-      </c>
-      <c r="N27">
-        <v>5700</v>
+        <v>600</v>
+      </c>
+      <c r="N27" t="s">
+        <v>30</v>
       </c>
       <c r="O27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P27" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>24</v>
+      </c>
+      <c r="R27" t="s">
         <v>26</v>
       </c>
-      <c r="Q27" t="s">
-        <v>26</v>
-      </c>
-      <c r="R27" t="s">
-        <v>27</v>
-      </c>
       <c r="S27" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="T27" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B28">
         <v>5.8</v>
@@ -2739,45 +2730,45 @@
         <v>8</v>
       </c>
       <c r="I28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K28" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M28">
         <v>600</v>
       </c>
       <c r="N28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S28" t="s">
+        <v>54</v>
+      </c>
+      <c r="T28" t="s">
         <v>119</v>
-      </c>
-      <c r="T28" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B29">
         <v>5.8</v>
@@ -2801,54 +2792,54 @@
         <v>8</v>
       </c>
       <c r="I29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K29" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L29" t="s">
-        <v>118</v>
+        <v>42</v>
       </c>
       <c r="M29">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="N29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S29" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="T29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B30">
-        <v>5.8</v>
+        <v>6.3</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30">
         <v>2</v>
@@ -2863,99 +2854,99 @@
         <v>8</v>
       </c>
       <c r="I30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J30" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="K30" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="L30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M30">
         <v>650</v>
       </c>
       <c r="N30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S30" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="T30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <v>8</v>
+      </c>
+      <c r="I31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" t="s">
+        <v>105</v>
+      </c>
+      <c r="K31" t="s">
         <v>125</v>
       </c>
-      <c r="B31">
-        <v>6.3</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31">
-        <v>2</v>
-      </c>
-      <c r="G31">
-        <v>8</v>
-      </c>
-      <c r="H31">
-        <v>8</v>
-      </c>
-      <c r="I31" t="s">
-        <v>31</v>
-      </c>
-      <c r="J31" t="s">
-        <v>32</v>
-      </c>
-      <c r="K31" t="s">
-        <v>103</v>
-      </c>
       <c r="L31" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="M31">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="N31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q31" t="s">
         <v>25</v>
       </c>
       <c r="R31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S31" t="s">
-        <v>119</v>
+        <v>54</v>
       </c>
       <c r="T31" t="s">
         <v>126</v>
@@ -2966,19 +2957,19 @@
         <v>127</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E32">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F32">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G32">
         <v>8</v>
@@ -2987,40 +2978,40 @@
         <v>8</v>
       </c>
       <c r="I32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J32" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="K32" t="s">
-        <v>128</v>
+        <v>37</v>
       </c>
       <c r="L32" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="M32">
-        <v>700</v>
+        <v>3000</v>
       </c>
       <c r="N32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P32" t="s">
         <v>25</v>
       </c>
       <c r="Q32" t="s">
+        <v>25</v>
+      </c>
+      <c r="R32" t="s">
         <v>26</v>
       </c>
-      <c r="R32" t="s">
-        <v>27</v>
-      </c>
       <c r="S32" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="T32" t="s">
-        <v>129</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -3028,128 +3019,128 @@
         <v>130</v>
       </c>
       <c r="B33">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="F33">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G33">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H33">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I33" t="s">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="J33" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="K33" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="L33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M33">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="N33" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="O33" t="s">
+        <v>24</v>
+      </c>
+      <c r="P33" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q33" t="s">
         <v>25</v>
       </c>
-      <c r="P33" t="s">
+      <c r="R33" t="s">
         <v>26</v>
       </c>
-      <c r="Q33" t="s">
-        <v>26</v>
-      </c>
-      <c r="R33" t="s">
-        <v>27</v>
-      </c>
       <c r="S33" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T33" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D34">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>10</v>
+        <v>5.5</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G34">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H34">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I34" t="s">
-        <v>134</v>
+        <v>20</v>
       </c>
       <c r="J34" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="K34" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L34" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="M34">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="N34" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="O34" t="s">
+        <v>24</v>
+      </c>
+      <c r="P34" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q34" t="s">
         <v>25</v>
       </c>
-      <c r="P34" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q34" t="s">
+      <c r="R34" t="s">
         <v>26</v>
       </c>
-      <c r="R34" t="s">
-        <v>27</v>
-      </c>
       <c r="S34" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="T34" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B35">
         <v>7.5</v>
@@ -3161,7 +3152,7 @@
         <v>10</v>
       </c>
       <c r="E35">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="F35">
         <v>3</v>
@@ -3173,45 +3164,45 @@
         <v>4</v>
       </c>
       <c r="I35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J35" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K35" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="L35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M35">
         <v>1000</v>
       </c>
       <c r="N35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O35" t="s">
+        <v>24</v>
+      </c>
+      <c r="P35" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q35" t="s">
         <v>25</v>
       </c>
-      <c r="P35" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q35" t="s">
+      <c r="R35" t="s">
         <v>26</v>
       </c>
-      <c r="R35" t="s">
-        <v>27</v>
-      </c>
       <c r="S35" t="s">
+        <v>137</v>
+      </c>
+      <c r="T35" t="s">
         <v>140</v>
-      </c>
-      <c r="T35" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B36">
         <v>7.5</v>
@@ -3223,7 +3214,7 @@
         <v>10</v>
       </c>
       <c r="E36">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="F36">
         <v>3</v>
@@ -3232,40 +3223,40 @@
         <v>5</v>
       </c>
       <c r="H36">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I36" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="J36" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K36" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="L36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M36">
-        <v>1000</v>
+        <v>1700</v>
       </c>
       <c r="N36" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O36" t="s">
         <v>25</v>
       </c>
       <c r="P36" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q36" t="s">
         <v>25</v>
       </c>
-      <c r="Q36" t="s">
-        <v>26</v>
-      </c>
       <c r="R36" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="S36" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="T36" t="s">
         <v>143</v>
@@ -3276,66 +3267,66 @@
         <v>144</v>
       </c>
       <c r="B37">
-        <v>7.5</v>
+        <v>6.6</v>
       </c>
       <c r="C37">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="D37">
         <v>10</v>
       </c>
       <c r="E37">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F37">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="G37">
         <v>5</v>
       </c>
       <c r="H37">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J37" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="K37" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="L37" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="M37">
-        <v>1700</v>
+        <v>1100</v>
       </c>
       <c r="N37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P37" t="s">
         <v>25</v>
       </c>
       <c r="Q37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="R37" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="S37" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="T37" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B38">
         <v>6.6</v>
@@ -3347,7 +3338,7 @@
         <v>10</v>
       </c>
       <c r="E38">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="F38">
         <v>9</v>
@@ -3359,34 +3350,34 @@
         <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J38" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L38" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M38">
-        <v>1100</v>
+        <v>1140</v>
       </c>
       <c r="N38" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="O38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q38" t="s">
         <v>25</v>
       </c>
       <c r="R38" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="S38" t="s">
         <v>150</v>
@@ -3397,58 +3388,58 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="B39">
-        <v>6.6</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="D39">
         <v>10</v>
       </c>
       <c r="E39">
-        <v>8.5</v>
+        <v>3.5</v>
       </c>
       <c r="F39">
-        <v>9</v>
+        <v>3.5</v>
       </c>
       <c r="G39">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I39" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="J39" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="K39" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="L39" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="M39">
-        <v>1140</v>
+        <v>2800</v>
       </c>
       <c r="N39" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="O39" t="s">
+        <v>24</v>
+      </c>
+      <c r="P39" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>24</v>
+      </c>
+      <c r="R39" t="s">
         <v>26</v>
-      </c>
-      <c r="P39" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>26</v>
-      </c>
-      <c r="R39" t="s">
-        <v>69</v>
       </c>
       <c r="S39" t="s">
         <v>153</v>
@@ -3483,60 +3474,60 @@
         <v>8</v>
       </c>
       <c r="I40" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K40" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="L40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M40">
         <v>2800</v>
       </c>
       <c r="N40" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O40" t="s">
+        <v>24</v>
+      </c>
+      <c r="P40" t="s">
         <v>25</v>
       </c>
-      <c r="P40" t="s">
+      <c r="Q40" t="s">
+        <v>24</v>
+      </c>
+      <c r="R40" t="s">
         <v>26</v>
       </c>
-      <c r="Q40" t="s">
-        <v>25</v>
-      </c>
-      <c r="R40" t="s">
-        <v>27</v>
-      </c>
       <c r="S40" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="T40" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41">
-        <v>8.5</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E41">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="F41">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="G41">
         <v>8</v>
@@ -3545,51 +3536,51 @@
         <v>8</v>
       </c>
       <c r="I41" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J41" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K41" t="s">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="L41" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="M41">
-        <v>2800</v>
+        <v>500</v>
       </c>
       <c r="N41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O41" t="s">
+        <v>24</v>
+      </c>
+      <c r="P41" t="s">
         <v>25</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
+        <v>24</v>
+      </c>
+      <c r="R41" t="s">
         <v>26</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>25</v>
-      </c>
-      <c r="R41" t="s">
-        <v>27</v>
       </c>
       <c r="S41" t="s">
         <v>157</v>
       </c>
       <c r="T41" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -3607,102 +3598,102 @@
         <v>8</v>
       </c>
       <c r="I42" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J42" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K42" t="s">
+        <v>51</v>
+      </c>
+      <c r="L42" t="s">
+        <v>42</v>
+      </c>
+      <c r="M42">
+        <v>1000</v>
+      </c>
+      <c r="N42" t="s">
+        <v>72</v>
+      </c>
+      <c r="O42" t="s">
+        <v>24</v>
+      </c>
+      <c r="P42" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>24</v>
+      </c>
+      <c r="R42" t="s">
+        <v>26</v>
+      </c>
+      <c r="S42" t="s">
+        <v>160</v>
+      </c>
+      <c r="T42" t="s">
         <v>54</v>
-      </c>
-      <c r="L42" t="s">
-        <v>24</v>
-      </c>
-      <c r="M42">
-        <v>500</v>
-      </c>
-      <c r="N42" t="s">
-        <v>75</v>
-      </c>
-      <c r="O42" t="s">
-        <v>25</v>
-      </c>
-      <c r="P42" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>25</v>
-      </c>
-      <c r="R42" t="s">
-        <v>27</v>
-      </c>
-      <c r="S42" t="s">
-        <v>161</v>
-      </c>
-      <c r="T42" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43">
+        <v>8.5</v>
+      </c>
+      <c r="C43">
+        <v>6.5</v>
+      </c>
+      <c r="D43">
+        <v>1.75</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>3</v>
+      </c>
+      <c r="I43" t="s">
+        <v>49</v>
+      </c>
+      <c r="J43" t="s">
+        <v>50</v>
+      </c>
+      <c r="K43" t="s">
+        <v>51</v>
+      </c>
+      <c r="L43" t="s">
+        <v>162</v>
+      </c>
+      <c r="M43">
+        <v>280</v>
+      </c>
+      <c r="N43" t="s">
+        <v>53</v>
+      </c>
+      <c r="O43" t="s">
+        <v>24</v>
+      </c>
+      <c r="P43" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>24</v>
+      </c>
+      <c r="R43" t="s">
+        <v>26</v>
+      </c>
+      <c r="S43" t="s">
         <v>163</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>2</v>
-      </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
-      <c r="F43">
-        <v>2</v>
-      </c>
-      <c r="G43">
-        <v>8</v>
-      </c>
-      <c r="H43">
-        <v>8</v>
-      </c>
-      <c r="I43" t="s">
-        <v>31</v>
-      </c>
-      <c r="J43" t="s">
-        <v>108</v>
-      </c>
-      <c r="K43" t="s">
-        <v>54</v>
-      </c>
-      <c r="L43" t="s">
-        <v>45</v>
-      </c>
-      <c r="M43">
-        <v>1000</v>
-      </c>
-      <c r="N43" t="s">
-        <v>75</v>
-      </c>
-      <c r="O43" t="s">
-        <v>25</v>
-      </c>
-      <c r="P43" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>25</v>
-      </c>
-      <c r="R43" t="s">
-        <v>27</v>
-      </c>
-      <c r="S43" t="s">
+      <c r="T43" t="s">
         <v>164</v>
-      </c>
-      <c r="T43" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -3713,10 +3704,10 @@
         <v>8.5</v>
       </c>
       <c r="C44">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="D44">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -3731,34 +3722,34 @@
         <v>3</v>
       </c>
       <c r="I44" t="s">
+        <v>49</v>
+      </c>
+      <c r="J44" t="s">
+        <v>166</v>
+      </c>
+      <c r="K44" t="s">
+        <v>51</v>
+      </c>
+      <c r="L44" t="s">
         <v>52</v>
       </c>
-      <c r="J44" t="s">
+      <c r="M44">
+        <v>300</v>
+      </c>
+      <c r="N44" t="s">
         <v>53</v>
       </c>
-      <c r="K44" t="s">
-        <v>54</v>
-      </c>
-      <c r="L44" t="s">
-        <v>166</v>
-      </c>
-      <c r="M44">
-        <v>280</v>
-      </c>
-      <c r="N44" t="s">
-        <v>56</v>
-      </c>
       <c r="O44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q44" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S44" t="s">
         <v>167</v>
@@ -3772,13 +3763,13 @@
         <v>169</v>
       </c>
       <c r="B45">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -3793,34 +3784,34 @@
         <v>3</v>
       </c>
       <c r="I45" t="s">
+        <v>49</v>
+      </c>
+      <c r="J45" t="s">
+        <v>96</v>
+      </c>
+      <c r="K45" t="s">
+        <v>170</v>
+      </c>
+      <c r="L45" t="s">
         <v>52</v>
       </c>
-      <c r="J45" t="s">
-        <v>170</v>
-      </c>
-      <c r="K45" t="s">
-        <v>54</v>
-      </c>
-      <c r="L45" t="s">
-        <v>55</v>
-      </c>
       <c r="M45">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="N45" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S45" t="s">
         <v>171</v>
@@ -3834,13 +3825,13 @@
         <v>173</v>
       </c>
       <c r="B46">
-        <v>9.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C46">
         <v>7.5</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -3855,99 +3846,99 @@
         <v>3</v>
       </c>
       <c r="I46" t="s">
+        <v>49</v>
+      </c>
+      <c r="J46" t="s">
+        <v>174</v>
+      </c>
+      <c r="K46" t="s">
+        <v>51</v>
+      </c>
+      <c r="L46" t="s">
         <v>52</v>
       </c>
-      <c r="J46" t="s">
-        <v>99</v>
-      </c>
-      <c r="K46" t="s">
-        <v>174</v>
-      </c>
-      <c r="L46" t="s">
-        <v>55</v>
-      </c>
       <c r="M46">
-        <v>600</v>
+        <v>830</v>
       </c>
       <c r="N46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S46" t="s">
+        <v>54</v>
+      </c>
+      <c r="T46" t="s">
         <v>175</v>
-      </c>
-      <c r="T46" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>176</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" t="s">
         <v>177</v>
       </c>
-      <c r="B47">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C47">
-        <v>7.5</v>
-      </c>
-      <c r="D47">
-        <v>2</v>
-      </c>
-      <c r="E47">
-        <v>2</v>
-      </c>
-      <c r="F47">
-        <v>2</v>
-      </c>
-      <c r="G47">
-        <v>3</v>
-      </c>
-      <c r="H47">
-        <v>3</v>
-      </c>
-      <c r="I47" t="s">
-        <v>52</v>
-      </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
+        <v>51</v>
+      </c>
+      <c r="L47" t="s">
+        <v>23</v>
+      </c>
+      <c r="M47">
+        <v>250</v>
+      </c>
+      <c r="N47" t="s">
+        <v>72</v>
+      </c>
+      <c r="O47" t="s">
+        <v>24</v>
+      </c>
+      <c r="P47" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>24</v>
+      </c>
+      <c r="R47" t="s">
+        <v>26</v>
+      </c>
+      <c r="S47" t="s">
         <v>178</v>
-      </c>
-      <c r="K47" t="s">
-        <v>54</v>
-      </c>
-      <c r="L47" t="s">
-        <v>55</v>
-      </c>
-      <c r="M47">
-        <v>830</v>
-      </c>
-      <c r="N47" t="s">
-        <v>56</v>
-      </c>
-      <c r="O47" t="s">
-        <v>25</v>
-      </c>
-      <c r="P47" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>25</v>
-      </c>
-      <c r="R47" t="s">
-        <v>27</v>
-      </c>
-      <c r="S47" t="s">
-        <v>57</v>
       </c>
       <c r="T47" t="s">
         <v>179</v>
@@ -3958,7 +3949,7 @@
         <v>180</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -3973,51 +3964,51 @@
         <v>2</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H48">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I48" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="J48" t="s">
+        <v>105</v>
+      </c>
+      <c r="K48" t="s">
+        <v>51</v>
+      </c>
+      <c r="L48" t="s">
+        <v>23</v>
+      </c>
+      <c r="M48">
+        <v>300</v>
+      </c>
+      <c r="N48" t="s">
+        <v>72</v>
+      </c>
+      <c r="O48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P48" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>24</v>
+      </c>
+      <c r="R48" t="s">
+        <v>26</v>
+      </c>
+      <c r="S48" t="s">
+        <v>178</v>
+      </c>
+      <c r="T48" t="s">
         <v>181</v>
-      </c>
-      <c r="K48" t="s">
-        <v>54</v>
-      </c>
-      <c r="L48" t="s">
-        <v>24</v>
-      </c>
-      <c r="M48">
-        <v>250</v>
-      </c>
-      <c r="N48" t="s">
-        <v>75</v>
-      </c>
-      <c r="O48" t="s">
-        <v>25</v>
-      </c>
-      <c r="P48" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>25</v>
-      </c>
-      <c r="R48" t="s">
-        <v>27</v>
-      </c>
-      <c r="S48" t="s">
-        <v>182</v>
-      </c>
-      <c r="T48" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -4041,51 +4032,51 @@
         <v>8</v>
       </c>
       <c r="I49" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J49" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K49" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M49">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="N49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S49" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T49" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -4097,51 +4088,51 @@
         <v>2</v>
       </c>
       <c r="G50">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H50">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I50" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="J50" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K50" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L50" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="M50">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="N50" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O50" t="s">
         <v>25</v>
       </c>
       <c r="P50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R50" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="S50" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="T50" t="s">
-        <v>185</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -4159,51 +4150,51 @@
         <v>2</v>
       </c>
       <c r="G51">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H51">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I51" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="J51" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L51" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="M51">
         <v>450</v>
       </c>
       <c r="N51" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O51" t="s">
+        <v>24</v>
+      </c>
+      <c r="P51" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>24</v>
+      </c>
+      <c r="R51" t="s">
         <v>26</v>
       </c>
-      <c r="P51" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>25</v>
-      </c>
-      <c r="R51" t="s">
-        <v>69</v>
-      </c>
       <c r="S51" t="s">
+        <v>186</v>
+      </c>
+      <c r="T51" t="s">
         <v>187</v>
-      </c>
-      <c r="T51" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -4221,51 +4212,51 @@
         <v>2</v>
       </c>
       <c r="G52">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H52">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I52" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="J52" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K52" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L52" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="M52">
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="N52" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O52" t="s">
         <v>25</v>
       </c>
       <c r="P52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R52" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="S52" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T52" t="s">
-        <v>191</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -4283,51 +4274,51 @@
         <v>2</v>
       </c>
       <c r="G53">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H53">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I53" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="J53" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K53" t="s">
+        <v>51</v>
+      </c>
+      <c r="L53" t="s">
+        <v>42</v>
+      </c>
+      <c r="M53">
+        <v>450</v>
+      </c>
+      <c r="N53" t="s">
+        <v>72</v>
+      </c>
+      <c r="O53" t="s">
+        <v>24</v>
+      </c>
+      <c r="P53" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>24</v>
+      </c>
+      <c r="R53" t="s">
+        <v>26</v>
+      </c>
+      <c r="S53" t="s">
         <v>54</v>
       </c>
-      <c r="L53" t="s">
-        <v>68</v>
-      </c>
-      <c r="M53">
-        <v>480</v>
-      </c>
-      <c r="N53" t="s">
-        <v>75</v>
-      </c>
-      <c r="O53" t="s">
-        <v>26</v>
-      </c>
-      <c r="P53" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>25</v>
-      </c>
-      <c r="R53" t="s">
-        <v>69</v>
-      </c>
-      <c r="S53" t="s">
-        <v>193</v>
-      </c>
       <c r="T53" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -4351,40 +4342,40 @@
         <v>8</v>
       </c>
       <c r="I54" t="s">
-        <v>31</v>
+        <v>192</v>
       </c>
       <c r="J54" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K54" t="s">
+        <v>51</v>
+      </c>
+      <c r="L54" t="s">
+        <v>115</v>
+      </c>
+      <c r="M54">
+        <v>600</v>
+      </c>
+      <c r="N54" t="s">
+        <v>72</v>
+      </c>
+      <c r="O54" t="s">
+        <v>24</v>
+      </c>
+      <c r="P54" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>24</v>
+      </c>
+      <c r="R54" t="s">
+        <v>193</v>
+      </c>
+      <c r="S54" t="s">
+        <v>194</v>
+      </c>
+      <c r="T54" t="s">
         <v>54</v>
-      </c>
-      <c r="L54" t="s">
-        <v>45</v>
-      </c>
-      <c r="M54">
-        <v>450</v>
-      </c>
-      <c r="N54" t="s">
-        <v>75</v>
-      </c>
-      <c r="O54" t="s">
-        <v>25</v>
-      </c>
-      <c r="P54" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>25</v>
-      </c>
-      <c r="R54" t="s">
-        <v>27</v>
-      </c>
-      <c r="S54" t="s">
-        <v>57</v>
-      </c>
-      <c r="T54" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
@@ -4398,7 +4389,7 @@
         <v>0</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -4413,40 +4404,40 @@
         <v>8</v>
       </c>
       <c r="I55" t="s">
+        <v>28</v>
+      </c>
+      <c r="J55" t="s">
+        <v>105</v>
+      </c>
+      <c r="K55" t="s">
         <v>196</v>
       </c>
-      <c r="J55" t="s">
-        <v>108</v>
-      </c>
-      <c r="K55" t="s">
-        <v>54</v>
-      </c>
       <c r="L55" t="s">
-        <v>118</v>
+        <v>23</v>
       </c>
       <c r="M55">
         <v>600</v>
       </c>
       <c r="N55" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R55" t="s">
+        <v>26</v>
+      </c>
+      <c r="S55" t="s">
         <v>197</v>
       </c>
-      <c r="S55" t="s">
+      <c r="T55" t="s">
         <v>198</v>
-      </c>
-      <c r="T55" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
@@ -4460,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="D56">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E56">
         <v>2</v>
@@ -4475,45 +4466,45 @@
         <v>8</v>
       </c>
       <c r="I56" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J56" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K56" t="s">
+        <v>51</v>
+      </c>
+      <c r="L56" t="s">
+        <v>42</v>
+      </c>
+      <c r="M56">
+        <v>700</v>
+      </c>
+      <c r="N56" t="s">
+        <v>72</v>
+      </c>
+      <c r="O56" t="s">
+        <v>24</v>
+      </c>
+      <c r="P56" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>24</v>
+      </c>
+      <c r="R56" t="s">
+        <v>26</v>
+      </c>
+      <c r="S56" t="s">
         <v>200</v>
       </c>
-      <c r="L56" t="s">
-        <v>24</v>
-      </c>
-      <c r="M56">
-        <v>600</v>
-      </c>
-      <c r="N56" t="s">
-        <v>75</v>
-      </c>
-      <c r="O56" t="s">
-        <v>25</v>
-      </c>
-      <c r="P56" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>25</v>
-      </c>
-      <c r="R56" t="s">
-        <v>27</v>
-      </c>
-      <c r="S56" t="s">
-        <v>201</v>
-      </c>
       <c r="T56" t="s">
-        <v>202</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -4522,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E57">
         <v>2</v>
@@ -4537,45 +4528,45 @@
         <v>8</v>
       </c>
       <c r="I57" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K57" t="s">
-        <v>54</v>
+        <v>196</v>
       </c>
       <c r="L57" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M57">
-        <v>700</v>
+        <v>850</v>
       </c>
       <c r="N57" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S57" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="T57" t="s">
-        <v>57</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -4587,238 +4578,176 @@
         <v>2.5</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="F58">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="G58">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H58">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I58" t="s">
-        <v>31</v>
+        <v>205</v>
       </c>
       <c r="J58" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K58" t="s">
-        <v>200</v>
+        <v>51</v>
       </c>
       <c r="L58" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="M58">
-        <v>850</v>
+        <v>1300</v>
       </c>
       <c r="N58" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S58" t="s">
         <v>206</v>
       </c>
       <c r="T58" t="s">
-        <v>207</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>5.8</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D59">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E59">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="F59">
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="G59">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H59">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I59" t="s">
-        <v>209</v>
+        <v>81</v>
       </c>
       <c r="J59" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="K59" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L59" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="M59">
-        <v>1300</v>
+        <v>1400</v>
       </c>
       <c r="N59" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O59" t="s">
         <v>25</v>
       </c>
       <c r="P59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R59" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="S59" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="T59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B60">
-        <v>5.8</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E60">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F60">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G60">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="H60">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>84</v>
+        <v>205</v>
       </c>
       <c r="J60" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="K60" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L60" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="M60">
-        <v>1400</v>
+        <v>1600</v>
       </c>
       <c r="N60" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O60" t="s">
+        <v>24</v>
+      </c>
+      <c r="P60" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>24</v>
+      </c>
+      <c r="R60" t="s">
         <v>26</v>
       </c>
-      <c r="P60" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>25</v>
-      </c>
-      <c r="R60" t="s">
-        <v>69</v>
-      </c>
       <c r="S60" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="T60" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>212</v>
-      </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-      <c r="D61">
-        <v>3</v>
-      </c>
-      <c r="E61">
-        <v>5</v>
-      </c>
-      <c r="F61">
-        <v>5</v>
-      </c>
-      <c r="G61">
-        <v>9</v>
-      </c>
-      <c r="H61">
-        <v>10</v>
-      </c>
-      <c r="I61" t="s">
-        <v>209</v>
-      </c>
-      <c r="J61" t="s">
-        <v>108</v>
-      </c>
-      <c r="K61" t="s">
-        <v>54</v>
-      </c>
-      <c r="L61" t="s">
-        <v>24</v>
-      </c>
-      <c r="M61">
-        <v>1600</v>
-      </c>
-      <c r="N61" t="s">
-        <v>75</v>
-      </c>
-      <c r="O61" t="s">
-        <v>25</v>
-      </c>
-      <c r="P61" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>25</v>
-      </c>
-      <c r="R61" t="s">
-        <v>27</v>
-      </c>
-      <c r="S61" t="s">
-        <v>213</v>
-      </c>
-      <c r="T61" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added subjective performance calculators
</commit_message>
<xml_diff>
--- a/data/monitors.xlsx
+++ b/data/monitors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandradeep/Desktop/MS/FrogAI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6ABB64-BEB2-E34F-B6C1-3499429273A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236E3473-B8DA-5647-9610-3526C7E3F66E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,9 +427,6 @@
     <t>W-OLED</t>
   </si>
   <si>
-    <t>Heavy matte coating + bad for text + burn in risk</t>
-  </si>
-  <si>
     <t>RTINGS,https://www.rtings.com/monitor/reviews/lg/27gr95qe-b;Hardware Unboxed,https://www.youtube.com/watch?v=2YBJFYGtmQk</t>
   </si>
   <si>
@@ -442,9 +439,6 @@
     <t>LG 45GR95QE</t>
   </si>
   <si>
-    <t>Heavy matte coating + low ppi + bad for text + burn in risk</t>
-  </si>
-  <si>
     <t>RTINGS,https://www.rtings.com/monitor/reviews/lg/45gr95qe-b</t>
   </si>
   <si>
@@ -457,18 +451,12 @@
     <t>QD-OLED</t>
   </si>
   <si>
-    <t>Broken HDR + bad for text + 3 year burn in warranty + glossy</t>
-  </si>
-  <si>
     <t>RTINGS,https://www.rtings.com/monitor/reviews/dell/alienware-aw3423dwf;Hardware Unboxed,https://www.youtube.com/watch?v=b0aLF3KVOTQ</t>
   </si>
   <si>
     <t>Alienware AW3423DW</t>
   </si>
   <si>
-    <t>Bad for text + 3 year burn in warranty + glossy</t>
-  </si>
-  <si>
     <t>RTINGS,https://www.rtings.com/monitor/reviews/dell/alienware-aw3423dw;Hardware Unboxed,https://www.youtube.com/watch?v=YleSuwK8vR4</t>
   </si>
   <si>
@@ -541,9 +529,6 @@
     <t>500hz</t>
   </si>
   <si>
-    <t>LTT,https://www.youtube.com/watch?v=Ewo8tt6bgZU</t>
-  </si>
-  <si>
     <t>Dell S2721D(S)</t>
   </si>
   <si>
@@ -656,6 +641,21 @@
   </si>
   <si>
     <t>OSD lock ups sometimes + minor VRR+HDR flickering</t>
+  </si>
+  <si>
+    <t>Heavy matte coating + burn in risk</t>
+  </si>
+  <si>
+    <t>Heavy matte coating + low ppi + burn in risk</t>
+  </si>
+  <si>
+    <t>Broken HDR+ 3 year burn in warranty + glossy</t>
+  </si>
+  <si>
+    <t>3 year burn in warranty + glossy</t>
+  </si>
+  <si>
+    <t>Linus Tech Tips,https://www.youtube.com/watch?v=Ewo8tt6bgZU;RTINGS,https://www.rtings.com/monitor/reviews/dell/alienware-aw2524h</t>
   </si>
 </sst>
 </file>
@@ -1021,14 +1021,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="S16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="19" max="19" width="30.6640625" customWidth="1"/>
+    <col min="19" max="19" width="61.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
@@ -1211,7 +1211,7 @@
         <v>26</v>
       </c>
       <c r="S3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="T3" t="s">
         <v>34</v>
@@ -1273,7 +1273,7 @@
         <v>26</v>
       </c>
       <c r="S4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="T4" t="s">
         <v>37</v>
@@ -1414,7 +1414,7 @@
         <v>6.5</v>
       </c>
       <c r="D7">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1600,7 +1600,7 @@
         <v>6.5</v>
       </c>
       <c r="D10">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1848,7 +1848,7 @@
         <v>6</v>
       </c>
       <c r="D14">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1910,7 +1910,7 @@
         <v>6.5</v>
       </c>
       <c r="D15">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -3100,7 +3100,7 @@
         <v>5</v>
       </c>
       <c r="H34">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I34" t="s">
         <v>20</v>
@@ -3133,15 +3133,15 @@
         <v>26</v>
       </c>
       <c r="S34" t="s">
+        <v>207</v>
+      </c>
+      <c r="T34" t="s">
         <v>135</v>
-      </c>
-      <c r="T34" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B35">
         <v>7.5</v>
@@ -3162,7 +3162,7 @@
         <v>5</v>
       </c>
       <c r="H35">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I35" t="s">
         <v>20</v>
@@ -3195,15 +3195,15 @@
         <v>26</v>
       </c>
       <c r="S35" t="s">
-        <v>135</v>
+        <v>207</v>
       </c>
       <c r="T35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B36">
         <v>7.5</v>
@@ -3257,15 +3257,15 @@
         <v>64</v>
       </c>
       <c r="S36" t="s">
-        <v>140</v>
+        <v>208</v>
       </c>
       <c r="T36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B37">
         <v>6.6</v>
@@ -3286,16 +3286,16 @@
         <v>5</v>
       </c>
       <c r="H37">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I37" t="s">
         <v>62</v>
       </c>
       <c r="J37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L37" t="s">
         <v>63</v>
@@ -3319,15 +3319,15 @@
         <v>64</v>
       </c>
       <c r="S37" t="s">
-        <v>145</v>
+        <v>209</v>
       </c>
       <c r="T37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B38">
         <v>6.6</v>
@@ -3348,16 +3348,16 @@
         <v>5</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="I38" t="s">
         <v>62</v>
       </c>
       <c r="J38" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L38" t="s">
         <v>63</v>
@@ -3381,15 +3381,15 @@
         <v>64</v>
       </c>
       <c r="S38" t="s">
-        <v>148</v>
+        <v>210</v>
       </c>
       <c r="T38" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -3419,7 +3419,7 @@
         <v>103</v>
       </c>
       <c r="K39" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L39" t="s">
         <v>40</v>
@@ -3443,15 +3443,15 @@
         <v>26</v>
       </c>
       <c r="S39" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="T39" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -3481,7 +3481,7 @@
         <v>103</v>
       </c>
       <c r="K40" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L40" t="s">
         <v>40</v>
@@ -3505,7 +3505,7 @@
         <v>26</v>
       </c>
       <c r="S40" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="T40" t="s">
         <v>52</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -3567,15 +3567,15 @@
         <v>26</v>
       </c>
       <c r="S41" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="T41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -3629,7 +3629,7 @@
         <v>26</v>
       </c>
       <c r="S42" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="T42" t="s">
         <v>52</v>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B43">
         <v>8.5</v>
@@ -3646,7 +3646,7 @@
         <v>6.5</v>
       </c>
       <c r="D43">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="E43">
         <v>2</v>
@@ -3670,7 +3670,7 @@
         <v>49</v>
       </c>
       <c r="L43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="M43">
         <v>280</v>
@@ -3691,15 +3691,15 @@
         <v>26</v>
       </c>
       <c r="S43" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="T43" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B44">
         <v>8.5</v>
@@ -3726,7 +3726,7 @@
         <v>47</v>
       </c>
       <c r="J44" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="K44" t="s">
         <v>49</v>
@@ -3753,15 +3753,15 @@
         <v>26</v>
       </c>
       <c r="S44" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="T44" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B45">
         <v>9.5</v>
@@ -3791,7 +3791,7 @@
         <v>94</v>
       </c>
       <c r="K45" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L45" t="s">
         <v>50</v>
@@ -3815,15 +3815,15 @@
         <v>26</v>
       </c>
       <c r="S45" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="T45" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B46">
         <v>8.8000000000000007</v>
@@ -3850,7 +3850,7 @@
         <v>47</v>
       </c>
       <c r="J46" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K46" t="s">
         <v>49</v>
@@ -3880,12 +3880,12 @@
         <v>52</v>
       </c>
       <c r="T46" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3912,7 +3912,7 @@
         <v>20</v>
       </c>
       <c r="J47" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K47" t="s">
         <v>49</v>
@@ -3939,15 +3939,15 @@
         <v>26</v>
       </c>
       <c r="S47" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="T47" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -4001,15 +4001,15 @@
         <v>26</v>
       </c>
       <c r="S48" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="T48" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -4063,15 +4063,15 @@
         <v>26</v>
       </c>
       <c r="S49" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="T49" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -4125,7 +4125,7 @@
         <v>64</v>
       </c>
       <c r="S50" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="T50" t="s">
         <v>52</v>
@@ -4133,7 +4133,7 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -4187,15 +4187,15 @@
         <v>26</v>
       </c>
       <c r="S51" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="T51" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -4249,7 +4249,7 @@
         <v>64</v>
       </c>
       <c r="S52" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="T52" t="s">
         <v>52</v>
@@ -4257,7 +4257,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -4319,7 +4319,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -4343,7 +4343,7 @@
         <v>8</v>
       </c>
       <c r="I54" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="J54" t="s">
         <v>103</v>
@@ -4370,10 +4370,10 @@
         <v>24</v>
       </c>
       <c r="R54" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="S54" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="T54" t="s">
         <v>52</v>
@@ -4381,7 +4381,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -4411,7 +4411,7 @@
         <v>103</v>
       </c>
       <c r="K55" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="L55" t="s">
         <v>23</v>
@@ -4435,15 +4435,15 @@
         <v>26</v>
       </c>
       <c r="S55" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="T55" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -4497,7 +4497,7 @@
         <v>26</v>
       </c>
       <c r="S56" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="T56" t="s">
         <v>52</v>
@@ -4505,7 +4505,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -4535,7 +4535,7 @@
         <v>103</v>
       </c>
       <c r="K57" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="L57" t="s">
         <v>40</v>
@@ -4559,15 +4559,15 @@
         <v>26</v>
       </c>
       <c r="S57" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="T57" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -4591,7 +4591,7 @@
         <v>10</v>
       </c>
       <c r="I58" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="J58" t="s">
         <v>103</v>
@@ -4621,7 +4621,7 @@
         <v>26</v>
       </c>
       <c r="S58" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="T58" t="s">
         <v>52</v>
@@ -4629,7 +4629,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B59">
         <v>5.8</v>
@@ -4683,7 +4683,7 @@
         <v>64</v>
       </c>
       <c r="S59" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="T59" t="s">
         <v>52</v>
@@ -4691,7 +4691,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4715,7 +4715,7 @@
         <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="J60" t="s">
         <v>103</v>
@@ -4745,10 +4745,10 @@
         <v>26</v>
       </c>
       <c r="S60" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="T60" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed light mdoe mobile bug
</commit_message>
<xml_diff>
--- a/data/monitors.xlsx
+++ b/data/monitors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandradeep/Desktop/MS/FrogAI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470E7D31-D562-E445-B5BC-9FBDB209F0A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E5E8A6-2454-294B-BD10-7FD1E9D92A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="29120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,9 +610,6 @@
     <t>Heavy matte coating + low ppi + burn in risk</t>
   </si>
   <si>
-    <t>Broken HDR+ 3 year burn in warranty + glossy</t>
-  </si>
-  <si>
     <t>3 year burn in warranty + glossy</t>
   </si>
   <si>
@@ -653,6 +650,9 @@
   </si>
   <si>
     <t>Needs to be warmed up for best motion performance</t>
+  </si>
+  <si>
+    <t>Broken HDR + 3 year burn in warranty + glossy</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1146,7 @@
         <v>26</v>
       </c>
       <c r="S2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T2" t="s">
         <v>31</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3">
         <v>7.5</v>
@@ -1208,7 +1208,7 @@
         <v>26</v>
       </c>
       <c r="S3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T3" t="s">
         <v>49</v>
@@ -1270,7 +1270,7 @@
         <v>26</v>
       </c>
       <c r="S4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T4" t="s">
         <v>33</v>
@@ -1332,7 +1332,7 @@
         <v>26</v>
       </c>
       <c r="S5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T5" t="s">
         <v>36</v>
@@ -1394,7 +1394,7 @@
         <v>26</v>
       </c>
       <c r="S6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="T6" t="s">
         <v>40</v>
@@ -1456,7 +1456,7 @@
         <v>26</v>
       </c>
       <c r="S7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="T7" t="s">
         <v>42</v>
@@ -3324,7 +3324,7 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B38">
         <v>6.6</v>
@@ -3378,7 +3378,7 @@
         <v>61</v>
       </c>
       <c r="S38" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="T38" t="s">
         <v>139</v>
@@ -3386,7 +3386,7 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39">
         <v>6.6</v>
@@ -3440,7 +3440,7 @@
         <v>61</v>
       </c>
       <c r="S39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T39" t="s">
         <v>140</v>
@@ -3750,7 +3750,7 @@
         <v>26</v>
       </c>
       <c r="S44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T44" t="s">
         <v>152</v>
@@ -3812,7 +3812,7 @@
         <v>26</v>
       </c>
       <c r="S45" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T45" t="s">
         <v>155</v>
@@ -3874,10 +3874,10 @@
         <v>26</v>
       </c>
       <c r="S46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="T46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added new monitors and fixed filters
</commit_message>
<xml_diff>
--- a/data/monitors.xlsx
+++ b/data/monitors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandradeep/Desktop/MS/FrogAI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14414B05-9FE7-BB44-A37A-A4B2A09CA81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712090A8-98B3-D040-98C5-DD2131AE35DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="248">
   <si>
     <t>name</t>
   </si>
@@ -716,6 +716,54 @@
   </si>
   <si>
     <t>[EU and UK only]</t>
+  </si>
+  <si>
+    <t>LG 32GQ850</t>
+  </si>
+  <si>
+    <t>260hz</t>
+  </si>
+  <si>
+    <t>270hz</t>
+  </si>
+  <si>
+    <t>Gigabyte FI32Q-X</t>
+  </si>
+  <si>
+    <t>Bijan Jamshidi,https://www.youtube.com/watch?v=-uv7io23Dsg</t>
+  </si>
+  <si>
+    <t>TFTCentral,https://tftcentral.co.uk/reviews/gigabyte-aorus-fi32q-x</t>
+  </si>
+  <si>
+    <t>Acer XB323U-GX</t>
+  </si>
+  <si>
+    <t>Same tuning and panel as 32GQ850</t>
+  </si>
+  <si>
+    <t>LG 42C2</t>
+  </si>
+  <si>
+    <t>42"</t>
+  </si>
+  <si>
+    <t>RTINGS,https://www.rtings.com/monitor/reviews/lg/42-c2-oled;Hardware Unboxed,https://www.youtube.com/watch?v=jRzGvkqSNaI</t>
+  </si>
+  <si>
+    <t>Sony Inzone M9</t>
+  </si>
+  <si>
+    <t>IPS FALD 96 zones</t>
+  </si>
+  <si>
+    <t>Very entry-level HDR and quite overpriced</t>
+  </si>
+  <si>
+    <t>RTINGS,https://www.rtings.com/monitor/reviews/sony/inzone-m9;Hardware Unboxed,https://www.youtube.com/watch?v=GNF2YMuITr0</t>
+  </si>
+  <si>
+    <t>Burn-in risk + glossy</t>
   </si>
 </sst>
 </file>
@@ -745,7 +793,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -768,15 +816,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,15 +1137,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T69"/>
+  <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="S73" sqref="S73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" customWidth="1"/>
     <col min="19" max="19" width="61.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3346,7 +3405,7 @@
         <v>5</v>
       </c>
       <c r="H37">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I37" t="s">
         <v>58</v>
@@ -5368,6 +5427,319 @@
       <c r="T69" t="s">
         <v>230</v>
       </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>232</v>
+      </c>
+      <c r="B70">
+        <v>7.7</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70">
+        <v>2</v>
+      </c>
+      <c r="G70">
+        <v>5</v>
+      </c>
+      <c r="H70">
+        <v>3</v>
+      </c>
+      <c r="I70" t="s">
+        <v>20</v>
+      </c>
+      <c r="J70" t="s">
+        <v>233</v>
+      </c>
+      <c r="K70" t="s">
+        <v>45</v>
+      </c>
+      <c r="L70" t="s">
+        <v>39</v>
+      </c>
+      <c r="M70">
+        <v>700</v>
+      </c>
+      <c r="N70">
+        <v>5700</v>
+      </c>
+      <c r="O70" t="s">
+        <v>24</v>
+      </c>
+      <c r="P70" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>24</v>
+      </c>
+      <c r="R70" t="s">
+        <v>26</v>
+      </c>
+      <c r="S70" t="s">
+        <v>48</v>
+      </c>
+      <c r="T70" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>235</v>
+      </c>
+      <c r="B71">
+        <v>7.8</v>
+      </c>
+      <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <v>5</v>
+      </c>
+      <c r="H71">
+        <v>3</v>
+      </c>
+      <c r="I71" t="s">
+        <v>20</v>
+      </c>
+      <c r="J71" t="s">
+        <v>234</v>
+      </c>
+      <c r="K71" t="s">
+        <v>45</v>
+      </c>
+      <c r="L71" t="s">
+        <v>39</v>
+      </c>
+      <c r="M71">
+        <v>700</v>
+      </c>
+      <c r="N71">
+        <v>5700</v>
+      </c>
+      <c r="O71" t="s">
+        <v>24</v>
+      </c>
+      <c r="P71" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>24</v>
+      </c>
+      <c r="R71" t="s">
+        <v>26</v>
+      </c>
+      <c r="S71" t="s">
+        <v>48</v>
+      </c>
+      <c r="T71" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>238</v>
+      </c>
+      <c r="B72">
+        <v>7.8</v>
+      </c>
+      <c r="C72">
+        <v>6</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+      <c r="F72">
+        <v>2</v>
+      </c>
+      <c r="G72">
+        <v>5</v>
+      </c>
+      <c r="H72">
+        <v>3</v>
+      </c>
+      <c r="I72" t="s">
+        <v>20</v>
+      </c>
+      <c r="J72" t="s">
+        <v>234</v>
+      </c>
+      <c r="K72" t="s">
+        <v>45</v>
+      </c>
+      <c r="L72" t="s">
+        <v>39</v>
+      </c>
+      <c r="M72">
+        <v>700</v>
+      </c>
+      <c r="N72">
+        <v>5700</v>
+      </c>
+      <c r="O72" t="s">
+        <v>24</v>
+      </c>
+      <c r="P72" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>24</v>
+      </c>
+      <c r="R72" t="s">
+        <v>26</v>
+      </c>
+      <c r="S72" t="s">
+        <v>239</v>
+      </c>
+      <c r="T72" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>240</v>
+      </c>
+      <c r="B73">
+        <v>5</v>
+      </c>
+      <c r="C73">
+        <v>9.5</v>
+      </c>
+      <c r="D73">
+        <v>10</v>
+      </c>
+      <c r="E73">
+        <v>7</v>
+      </c>
+      <c r="F73">
+        <v>3.5</v>
+      </c>
+      <c r="G73">
+        <v>8</v>
+      </c>
+      <c r="H73">
+        <v>1.5</v>
+      </c>
+      <c r="I73" t="s">
+        <v>28</v>
+      </c>
+      <c r="J73" t="s">
+        <v>122</v>
+      </c>
+      <c r="K73" t="s">
+        <v>130</v>
+      </c>
+      <c r="L73" t="s">
+        <v>241</v>
+      </c>
+      <c r="M73">
+        <v>1000</v>
+      </c>
+      <c r="N73" t="s">
+        <v>30</v>
+      </c>
+      <c r="O73" t="s">
+        <v>24</v>
+      </c>
+      <c r="P73" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>25</v>
+      </c>
+      <c r="R73" t="s">
+        <v>26</v>
+      </c>
+      <c r="S73" t="s">
+        <v>247</v>
+      </c>
+      <c r="T73" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>243</v>
+      </c>
+      <c r="B74">
+        <v>5.8</v>
+      </c>
+      <c r="C74">
+        <v>6.2</v>
+      </c>
+      <c r="D74">
+        <v>4</v>
+      </c>
+      <c r="E74">
+        <v>6.1</v>
+      </c>
+      <c r="F74">
+        <v>4</v>
+      </c>
+      <c r="G74">
+        <v>8</v>
+      </c>
+      <c r="H74">
+        <v>8</v>
+      </c>
+      <c r="I74" t="s">
+        <v>28</v>
+      </c>
+      <c r="J74" t="s">
+        <v>38</v>
+      </c>
+      <c r="K74" t="s">
+        <v>244</v>
+      </c>
+      <c r="L74" t="s">
+        <v>23</v>
+      </c>
+      <c r="M74">
+        <v>900</v>
+      </c>
+      <c r="N74" t="s">
+        <v>30</v>
+      </c>
+      <c r="O74" t="s">
+        <v>24</v>
+      </c>
+      <c r="P74" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>24</v>
+      </c>
+      <c r="R74" t="s">
+        <v>26</v>
+      </c>
+      <c r="S74" t="s">
+        <v>245</v>
+      </c>
+      <c r="T74" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E78" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated due to ULMB2
</commit_message>
<xml_diff>
--- a/data/monitors.xlsx
+++ b/data/monitors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chandradeep/Desktop/MS/FrogAI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8C3F0E-D59C-EE49-94C6-6E05435E074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC80FB4D-CD83-794D-A484-D37A613EF733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20560" yWindow="880" windowWidth="20560" windowHeight="25700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="244">
   <si>
     <t>name</t>
   </si>
@@ -289,9 +289,6 @@
     <t>360hz</t>
   </si>
   <si>
-    <t>RTINGS,https://www.rtings.com/monitor/reviews/asus/rog-swift-360hz-pg27aqn;Hardware Unboxed,https://www.youtube.com/watch?v=eYFtLBM3a78</t>
-  </si>
-  <si>
     <t>Dell S2722DGM</t>
   </si>
   <si>
@@ -733,9 +730,6 @@
     <t>Asus XB273U F</t>
   </si>
   <si>
-    <t>Gsync module + slightly cheaper version of PG27AQN</t>
-  </si>
-  <si>
     <t>VRR+HDR flickering + might have to wait for restock + Type-c hub with 90W charging</t>
   </si>
   <si>
@@ -749,6 +743,15 @@
   </si>
   <si>
     <t>Reports of coil whine + Type-c hub with 90W charging + might have to wait for restock</t>
+  </si>
+  <si>
+    <t>Gsync module + ULMB2</t>
+  </si>
+  <si>
+    <t>Gsync module + ULMB2 + slightly cheaper version of PG27AQN</t>
+  </si>
+  <si>
+    <t>RTINGS,https://www.rtings.com/monitor/reviews/asus/rog-swift-360hz-pg27aqn;Hardware Unboxed,https://www.youtube.com/watch?v=eYFtLBM3a78;Optimum Tech,https://www.youtube.com/watch?v=3Cykx2GQq4k</t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" topLeftCell="Y53" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AH75" sqref="AH75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1253,7 +1256,7 @@
         <v>26</v>
       </c>
       <c r="S2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="T2" t="s">
         <v>31</v>
@@ -1261,7 +1264,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3">
         <v>7.5</v>
@@ -1291,7 +1294,7 @@
         <v>44</v>
       </c>
       <c r="K3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L3" t="s">
         <v>23</v>
@@ -1315,7 +1318,7 @@
         <v>26</v>
       </c>
       <c r="S3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T3" t="s">
         <v>48</v>
@@ -1377,7 +1380,7 @@
         <v>26</v>
       </c>
       <c r="S4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="T4" t="s">
         <v>33</v>
@@ -1439,7 +1442,7 @@
         <v>26</v>
       </c>
       <c r="S5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="T5" t="s">
         <v>36</v>
@@ -1501,7 +1504,7 @@
         <v>26</v>
       </c>
       <c r="S6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="T6" t="s">
         <v>40</v>
@@ -1509,7 +1512,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7">
         <v>6.25</v>
@@ -1563,7 +1566,7 @@
         <v>26</v>
       </c>
       <c r="S7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="T7" t="s">
         <v>41</v>
@@ -1625,7 +1628,7 @@
         <v>26</v>
       </c>
       <c r="S8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="T8" t="s">
         <v>49</v>
@@ -2067,7 +2070,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B16">
         <v>5.8</v>
@@ -2183,7 +2186,7 @@
         <v>60</v>
       </c>
       <c r="S17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="T17" t="s">
         <v>76</v>
@@ -2431,7 +2434,7 @@
         <v>26</v>
       </c>
       <c r="S21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="T21" t="s">
         <v>86</v>
@@ -2442,7 +2445,7 @@
         <v>87</v>
       </c>
       <c r="B22">
-        <v>8.3000000000000007</v>
+        <v>9.75</v>
       </c>
       <c r="C22">
         <v>8</v>
@@ -2493,15 +2496,15 @@
         <v>26</v>
       </c>
       <c r="S22" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="T22" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23">
         <v>6.3</v>
@@ -2531,7 +2534,7 @@
         <v>21</v>
       </c>
       <c r="K23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
@@ -2558,12 +2561,12 @@
         <v>48</v>
       </c>
       <c r="T23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24">
         <v>6.3</v>
@@ -2593,7 +2596,7 @@
         <v>21</v>
       </c>
       <c r="K24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L24" t="s">
         <v>39</v>
@@ -2620,12 +2623,12 @@
         <v>48</v>
       </c>
       <c r="T24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2652,10 +2655,10 @@
         <v>28</v>
       </c>
       <c r="J25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L25" t="s">
         <v>39</v>
@@ -2682,12 +2685,12 @@
         <v>48</v>
       </c>
       <c r="T25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26">
         <v>5.8</v>
@@ -2717,7 +2720,7 @@
         <v>38</v>
       </c>
       <c r="K26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L26" t="s">
         <v>59</v>
@@ -2726,7 +2729,7 @@
         <v>450</v>
       </c>
       <c r="N26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O26" t="s">
         <v>25</v>
@@ -2741,15 +2744,15 @@
         <v>60</v>
       </c>
       <c r="S26" t="s">
+        <v>99</v>
+      </c>
+      <c r="T26" t="s">
         <v>100</v>
-      </c>
-      <c r="T26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27">
         <v>6.3</v>
@@ -2779,7 +2782,7 @@
         <v>21</v>
       </c>
       <c r="K27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L27" t="s">
         <v>23</v>
@@ -2803,15 +2806,15 @@
         <v>26</v>
       </c>
       <c r="S27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28">
         <v>5.8</v>
@@ -2844,7 +2847,7 @@
         <v>45</v>
       </c>
       <c r="L28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M28">
         <v>600</v>
@@ -2865,15 +2868,15 @@
         <v>26</v>
       </c>
       <c r="S28" t="s">
+        <v>106</v>
+      </c>
+      <c r="T28" t="s">
         <v>107</v>
-      </c>
-      <c r="T28" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29">
         <v>5.8</v>
@@ -2906,7 +2909,7 @@
         <v>45</v>
       </c>
       <c r="L29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M29">
         <v>600</v>
@@ -2930,12 +2933,12 @@
         <v>48</v>
       </c>
       <c r="T29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30">
         <v>5.8</v>
@@ -2989,15 +2992,15 @@
         <v>26</v>
       </c>
       <c r="S30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31">
         <v>6.3</v>
@@ -3027,7 +3030,7 @@
         <v>29</v>
       </c>
       <c r="K31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L31" t="s">
         <v>39</v>
@@ -3051,15 +3054,15 @@
         <v>26</v>
       </c>
       <c r="S31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -3086,10 +3089,10 @@
         <v>28</v>
       </c>
       <c r="J32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L32" t="s">
         <v>23</v>
@@ -3116,12 +3119,12 @@
         <v>48</v>
       </c>
       <c r="T32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33">
         <v>5</v>
@@ -3148,7 +3151,7 @@
         <v>28</v>
       </c>
       <c r="J33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K33" t="s">
         <v>35</v>
@@ -3175,7 +3178,7 @@
         <v>26</v>
       </c>
       <c r="S33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="T33" t="s">
         <v>48</v>
@@ -3183,7 +3186,7 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -3207,13 +3210,13 @@
         <v>10</v>
       </c>
       <c r="I34" t="s">
+        <v>121</v>
+      </c>
+      <c r="J34" t="s">
+        <v>95</v>
+      </c>
+      <c r="K34" t="s">
         <v>122</v>
-      </c>
-      <c r="J34" t="s">
-        <v>96</v>
-      </c>
-      <c r="K34" t="s">
-        <v>123</v>
       </c>
       <c r="L34" t="s">
         <v>39</v>
@@ -3237,15 +3240,15 @@
         <v>26</v>
       </c>
       <c r="S34" t="s">
+        <v>123</v>
+      </c>
+      <c r="T34" t="s">
         <v>124</v>
-      </c>
-      <c r="T34" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35">
         <v>7.5</v>
@@ -3275,7 +3278,7 @@
         <v>44</v>
       </c>
       <c r="K35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L35" t="s">
         <v>23</v>
@@ -3299,15 +3302,15 @@
         <v>26</v>
       </c>
       <c r="S35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="T35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B36">
         <v>7.5</v>
@@ -3337,7 +3340,7 @@
         <v>44</v>
       </c>
       <c r="K36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L36" t="s">
         <v>23</v>
@@ -3361,15 +3364,15 @@
         <v>26</v>
       </c>
       <c r="S36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="T36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B37">
         <v>7.5</v>
@@ -3399,7 +3402,7 @@
         <v>44</v>
       </c>
       <c r="K37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L37" t="s">
         <v>23</v>
@@ -3423,15 +3426,15 @@
         <v>60</v>
       </c>
       <c r="S37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B38">
         <v>6.6</v>
@@ -3458,10 +3461,10 @@
         <v>58</v>
       </c>
       <c r="J38" t="s">
+        <v>132</v>
+      </c>
+      <c r="K38" t="s">
         <v>133</v>
-      </c>
-      <c r="K38" t="s">
-        <v>134</v>
       </c>
       <c r="L38" t="s">
         <v>59</v>
@@ -3485,15 +3488,15 @@
         <v>60</v>
       </c>
       <c r="S38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B39">
         <v>6.6</v>
@@ -3520,10 +3523,10 @@
         <v>58</v>
       </c>
       <c r="J39" t="s">
+        <v>132</v>
+      </c>
+      <c r="K39" t="s">
         <v>133</v>
-      </c>
-      <c r="K39" t="s">
-        <v>134</v>
       </c>
       <c r="L39" t="s">
         <v>59</v>
@@ -3547,15 +3550,15 @@
         <v>60</v>
       </c>
       <c r="S39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="T39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -3582,10 +3585,10 @@
         <v>28</v>
       </c>
       <c r="J40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L40" t="s">
         <v>39</v>
@@ -3609,15 +3612,15 @@
         <v>26</v>
       </c>
       <c r="S40" t="s">
+        <v>137</v>
+      </c>
+      <c r="T40" t="s">
         <v>138</v>
-      </c>
-      <c r="T40" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -3644,10 +3647,10 @@
         <v>28</v>
       </c>
       <c r="J41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L41" t="s">
         <v>39</v>
@@ -3671,7 +3674,7 @@
         <v>26</v>
       </c>
       <c r="S41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T41" t="s">
         <v>48</v>
@@ -3679,7 +3682,7 @@
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -3706,7 +3709,7 @@
         <v>28</v>
       </c>
       <c r="J42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K42" t="s">
         <v>45</v>
@@ -3733,15 +3736,15 @@
         <v>26</v>
       </c>
       <c r="S42" t="s">
+        <v>141</v>
+      </c>
+      <c r="T42" t="s">
         <v>142</v>
-      </c>
-      <c r="T42" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -3768,7 +3771,7 @@
         <v>28</v>
       </c>
       <c r="J43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K43" t="s">
         <v>45</v>
@@ -3795,7 +3798,7 @@
         <v>26</v>
       </c>
       <c r="S43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T43" t="s">
         <v>48</v>
@@ -3803,7 +3806,7 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B44">
         <v>8.5</v>
@@ -3836,7 +3839,7 @@
         <v>45</v>
       </c>
       <c r="L44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M44">
         <v>280</v>
@@ -3857,15 +3860,15 @@
         <v>26</v>
       </c>
       <c r="S44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="T44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B45">
         <v>9.5</v>
@@ -3895,7 +3898,7 @@
         <v>88</v>
       </c>
       <c r="K45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L45" t="s">
         <v>46</v>
@@ -3919,15 +3922,15 @@
         <v>26</v>
       </c>
       <c r="S45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="T45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B46">
         <v>8.8000000000000007</v>
@@ -3954,7 +3957,7 @@
         <v>43</v>
       </c>
       <c r="J46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K46" t="s">
         <v>45</v>
@@ -3981,15 +3984,15 @@
         <v>26</v>
       </c>
       <c r="S46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -4016,7 +4019,7 @@
         <v>20</v>
       </c>
       <c r="J47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K47" t="s">
         <v>45</v>
@@ -4043,15 +4046,15 @@
         <v>26</v>
       </c>
       <c r="S47" t="s">
+        <v>155</v>
+      </c>
+      <c r="T47" t="s">
         <v>156</v>
-      </c>
-      <c r="T47" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -4078,7 +4081,7 @@
         <v>28</v>
       </c>
       <c r="J48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K48" t="s">
         <v>45</v>
@@ -4105,15 +4108,15 @@
         <v>26</v>
       </c>
       <c r="S48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="T48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -4140,7 +4143,7 @@
         <v>28</v>
       </c>
       <c r="J49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K49" t="s">
         <v>45</v>
@@ -4167,15 +4170,15 @@
         <v>26</v>
       </c>
       <c r="S49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -4202,7 +4205,7 @@
         <v>58</v>
       </c>
       <c r="J50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K50" t="s">
         <v>45</v>
@@ -4229,7 +4232,7 @@
         <v>60</v>
       </c>
       <c r="S50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T50" t="s">
         <v>48</v>
@@ -4237,7 +4240,7 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -4264,7 +4267,7 @@
         <v>28</v>
       </c>
       <c r="J51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K51" t="s">
         <v>45</v>
@@ -4291,15 +4294,15 @@
         <v>26</v>
       </c>
       <c r="S51" t="s">
+        <v>163</v>
+      </c>
+      <c r="T51" t="s">
         <v>164</v>
-      </c>
-      <c r="T51" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -4326,7 +4329,7 @@
         <v>58</v>
       </c>
       <c r="J52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K52" t="s">
         <v>45</v>
@@ -4353,7 +4356,7 @@
         <v>60</v>
       </c>
       <c r="S52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T52" t="s">
         <v>48</v>
@@ -4361,7 +4364,7 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -4388,7 +4391,7 @@
         <v>28</v>
       </c>
       <c r="J53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K53" t="s">
         <v>45</v>
@@ -4423,7 +4426,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -4447,16 +4450,16 @@
         <v>8</v>
       </c>
       <c r="I54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K54" t="s">
         <v>45</v>
       </c>
       <c r="L54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M54">
         <v>600</v>
@@ -4474,10 +4477,10 @@
         <v>24</v>
       </c>
       <c r="R54" t="s">
+        <v>170</v>
+      </c>
+      <c r="S54" t="s">
         <v>171</v>
-      </c>
-      <c r="S54" t="s">
-        <v>172</v>
       </c>
       <c r="T54" t="s">
         <v>48</v>
@@ -4485,7 +4488,7 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -4512,10 +4515,10 @@
         <v>28</v>
       </c>
       <c r="J55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L55" t="s">
         <v>23</v>
@@ -4539,15 +4542,15 @@
         <v>26</v>
       </c>
       <c r="S55" t="s">
+        <v>174</v>
+      </c>
+      <c r="T55" t="s">
         <v>175</v>
-      </c>
-      <c r="T55" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -4574,7 +4577,7 @@
         <v>28</v>
       </c>
       <c r="J56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K56" t="s">
         <v>45</v>
@@ -4601,7 +4604,7 @@
         <v>26</v>
       </c>
       <c r="S56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T56" t="s">
         <v>48</v>
@@ -4609,7 +4612,7 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -4636,10 +4639,10 @@
         <v>28</v>
       </c>
       <c r="J57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K57" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L57" t="s">
         <v>39</v>
@@ -4663,15 +4666,15 @@
         <v>26</v>
       </c>
       <c r="S57" t="s">
+        <v>179</v>
+      </c>
+      <c r="T57" t="s">
         <v>180</v>
-      </c>
-      <c r="T57" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -4695,10 +4698,10 @@
         <v>10</v>
       </c>
       <c r="I58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K58" t="s">
         <v>45</v>
@@ -4725,7 +4728,7 @@
         <v>26</v>
       </c>
       <c r="S58" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="T58" t="s">
         <v>48</v>
@@ -4733,7 +4736,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B59">
         <v>5.8</v>
@@ -4787,7 +4790,7 @@
         <v>60</v>
       </c>
       <c r="S59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T59" t="s">
         <v>48</v>
@@ -4795,7 +4798,7 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4819,10 +4822,10 @@
         <v>10</v>
       </c>
       <c r="I60" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K60" t="s">
         <v>45</v>
@@ -4849,15 +4852,15 @@
         <v>26</v>
       </c>
       <c r="S60" t="s">
+        <v>186</v>
+      </c>
+      <c r="T60" t="s">
         <v>187</v>
-      </c>
-      <c r="T60" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B61">
         <v>6.6</v>
@@ -4914,12 +4917,12 @@
         <v>48</v>
       </c>
       <c r="T61" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B62">
         <v>6.25</v>
@@ -4976,12 +4979,12 @@
         <v>48</v>
       </c>
       <c r="T62" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B63">
         <v>6.4</v>
@@ -5014,7 +5017,7 @@
         <v>45</v>
       </c>
       <c r="L63" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M63">
         <v>150</v>
@@ -5035,15 +5038,15 @@
         <v>26</v>
       </c>
       <c r="S63" t="s">
+        <v>204</v>
+      </c>
+      <c r="T63" t="s">
         <v>205</v>
-      </c>
-      <c r="T63" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B64">
         <v>6.3</v>
@@ -5076,7 +5079,7 @@
         <v>45</v>
       </c>
       <c r="L64" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M64">
         <v>200</v>
@@ -5100,12 +5103,12 @@
         <v>48</v>
       </c>
       <c r="T64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B65">
         <v>6.3</v>
@@ -5138,7 +5141,7 @@
         <v>45</v>
       </c>
       <c r="L65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M65">
         <v>190</v>
@@ -5167,7 +5170,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B66">
         <v>7.7</v>
@@ -5194,7 +5197,7 @@
         <v>20</v>
       </c>
       <c r="J66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K66" t="s">
         <v>45</v>
@@ -5224,12 +5227,12 @@
         <v>48</v>
       </c>
       <c r="T66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B67">
         <v>7.8</v>
@@ -5256,7 +5259,7 @@
         <v>20</v>
       </c>
       <c r="J67" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K67" t="s">
         <v>45</v>
@@ -5286,12 +5289,12 @@
         <v>48</v>
       </c>
       <c r="T67" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B68">
         <v>7.8</v>
@@ -5318,7 +5321,7 @@
         <v>20</v>
       </c>
       <c r="J68" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K68" t="s">
         <v>45</v>
@@ -5345,7 +5348,7 @@
         <v>26</v>
       </c>
       <c r="S68" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="T68" t="s">
         <v>48</v>
@@ -5353,7 +5356,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B69">
         <v>5</v>
@@ -5380,13 +5383,13 @@
         <v>28</v>
       </c>
       <c r="J69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L69" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="M69">
         <v>1000</v>
@@ -5407,15 +5410,15 @@
         <v>26</v>
       </c>
       <c r="S69" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="T69" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B70">
         <v>5.8</v>
@@ -5445,7 +5448,7 @@
         <v>38</v>
       </c>
       <c r="K70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L70" t="s">
         <v>23</v>
@@ -5469,15 +5472,15 @@
         <v>26</v>
       </c>
       <c r="S70" t="s">
+        <v>223</v>
+      </c>
+      <c r="T70" t="s">
         <v>224</v>
-      </c>
-      <c r="T70" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B71">
         <v>6.4</v>
@@ -5531,7 +5534,7 @@
         <v>26</v>
       </c>
       <c r="S71" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="T71" t="s">
         <v>54</v>
@@ -5539,13 +5542,13 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B72">
-        <v>8.3000000000000007</v>
+        <v>9.75</v>
       </c>
       <c r="C72">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="D72">
         <v>2</v>
@@ -5593,10 +5596,10 @@
         <v>26</v>
       </c>
       <c r="S72" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="T72" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>